<commit_message>
Has bugs when inserting in database
The datestamp is missing from some variables and there seems to be a problem in Mixintables.add whith the transformer
</commit_message>
<xml_diff>
--- a/dados/Template SE8.xlsx
+++ b/dados/Template SE8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Documents\SEAI---Equipa-F\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E319D3-767B-48DC-8D8E-02629C7B7541}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D355C4D3-B974-4877-86A3-4D12AD580E35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DGA" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="214">
   <si>
     <t>Samples</t>
   </si>
@@ -565,48 +565,6 @@
   </si>
   <si>
     <t>dez</t>
-  </si>
-  <si>
-    <t>DATA.XL</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>11,9</t>
-  </si>
-  <si>
-    <t>3,2</t>
-  </si>
-  <si>
-    <t>2,2</t>
-  </si>
-  <si>
-    <t>2,9</t>
-  </si>
-  <si>
-    <t>175,9</t>
-  </si>
-  <si>
-    <t>3,46</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>&lt; 1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>216</t>
-  </si>
-  <si>
-    <t>3,54</t>
   </si>
   <si>
     <t>foi o 2fal</t>
@@ -2210,14 +2168,6 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection hidden="1"/>
@@ -2230,47 +2180,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -2295,6 +2205,54 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -7680,8 +7638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ37"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J35" sqref="C17:J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8257,533 +8215,229 @@
       <c r="G13" s="20"/>
     </row>
     <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="3:15" ht="44.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="156" t="s">
-        <v>173</v>
-      </c>
-      <c r="D17" s="156" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="156" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="157" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="156" t="s">
-        <v>9</v>
-      </c>
-      <c r="H17" s="156" t="s">
-        <v>11</v>
-      </c>
-      <c r="I17" s="156" t="s">
-        <v>13</v>
-      </c>
-      <c r="J17" s="156" t="s">
-        <v>15</v>
-      </c>
+    <row r="17" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="156"/>
+      <c r="D17" s="156"/>
+      <c r="E17" s="156"/>
+      <c r="F17" s="157"/>
+      <c r="G17" s="156"/>
+      <c r="H17" s="156"/>
+      <c r="I17" s="156"/>
+      <c r="J17" s="156"/>
       <c r="N17" s="142"/>
       <c r="O17" s="142"/>
     </row>
     <row r="18" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="150">
-        <v>42333.395833333336</v>
-      </c>
-      <c r="D18" s="151" t="s">
-        <v>182</v>
-      </c>
-      <c r="E18" s="151" t="s">
-        <v>185</v>
-      </c>
-      <c r="F18" s="151" t="s">
-        <v>186</v>
-      </c>
-      <c r="G18" s="151" t="s">
-        <v>174</v>
-      </c>
-      <c r="H18" s="151" t="s">
-        <v>183</v>
-      </c>
-      <c r="I18" s="151" t="s">
-        <v>184</v>
-      </c>
-      <c r="J18" s="151" t="s">
-        <v>183</v>
-      </c>
+      <c r="C18" s="150"/>
+      <c r="D18" s="151"/>
+      <c r="E18" s="151"/>
+      <c r="F18" s="151"/>
+      <c r="G18" s="151"/>
+      <c r="H18" s="151"/>
+      <c r="I18" s="151"/>
+      <c r="J18" s="151"/>
       <c r="N18" s="143"/>
       <c r="O18" s="143"/>
     </row>
     <row r="19" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="150">
-        <v>41710</v>
-      </c>
-      <c r="D19" s="151" t="s">
-        <v>176</v>
-      </c>
-      <c r="E19" s="151" t="s">
-        <v>180</v>
-      </c>
-      <c r="F19" s="151" t="s">
-        <v>181</v>
-      </c>
-      <c r="G19" s="151" t="s">
-        <v>177</v>
-      </c>
-      <c r="H19" s="151" t="s">
-        <v>178</v>
-      </c>
-      <c r="I19" s="151" t="s">
-        <v>179</v>
-      </c>
-      <c r="J19" s="151" t="s">
-        <v>175</v>
-      </c>
+      <c r="C19" s="150"/>
+      <c r="D19" s="151"/>
+      <c r="E19" s="151"/>
+      <c r="F19" s="151"/>
+      <c r="G19" s="151"/>
+      <c r="H19" s="151"/>
+      <c r="I19" s="151"/>
+      <c r="J19" s="151"/>
       <c r="N19" s="143"/>
       <c r="O19" s="143"/>
     </row>
     <row r="20" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="150">
-        <v>40254</v>
-      </c>
-      <c r="D20" s="152">
-        <v>3.4</v>
-      </c>
-      <c r="E20" s="152">
-        <v>132.6</v>
-      </c>
-      <c r="F20" s="154">
-        <v>4.93</v>
-      </c>
-      <c r="G20" s="152">
-        <v>2.8</v>
-      </c>
-      <c r="H20" s="152">
-        <v>1</v>
-      </c>
-      <c r="I20" s="152">
-        <v>3</v>
-      </c>
-      <c r="J20" s="152">
-        <v>0</v>
-      </c>
+      <c r="C20" s="150"/>
+      <c r="D20" s="152"/>
+      <c r="E20" s="152"/>
+      <c r="F20" s="154"/>
+      <c r="G20" s="152"/>
+      <c r="H20" s="152"/>
+      <c r="I20" s="152"/>
+      <c r="J20" s="152"/>
       <c r="N20" s="144"/>
       <c r="O20" s="144"/>
     </row>
     <row r="21" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="150">
-        <v>39850</v>
-      </c>
-      <c r="D21" s="152">
-        <v>8.6</v>
-      </c>
-      <c r="E21" s="152">
-        <v>327</v>
-      </c>
-      <c r="F21" s="154">
-        <v>6.35</v>
-      </c>
-      <c r="G21" s="152">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="H21" s="152">
-        <v>1.6</v>
-      </c>
-      <c r="I21" s="152">
-        <v>3.4</v>
-      </c>
-      <c r="J21" s="152">
-        <v>0</v>
-      </c>
+      <c r="C21" s="150"/>
+      <c r="D21" s="152"/>
+      <c r="E21" s="152"/>
+      <c r="F21" s="154"/>
+      <c r="G21" s="152"/>
+      <c r="H21" s="152"/>
+      <c r="I21" s="152"/>
+      <c r="J21" s="152"/>
       <c r="N21" s="144"/>
       <c r="O21" s="144"/>
     </row>
     <row r="22" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="150">
-        <v>39547</v>
-      </c>
-      <c r="D22" s="152">
-        <v>12.3</v>
-      </c>
-      <c r="E22" s="152">
-        <v>355.5</v>
-      </c>
-      <c r="F22" s="154">
-        <v>7.62</v>
-      </c>
-      <c r="G22" s="152">
-        <v>4.2</v>
-      </c>
-      <c r="H22" s="152">
-        <v>1.6</v>
-      </c>
-      <c r="I22" s="152">
-        <v>3.6</v>
-      </c>
-      <c r="J22" s="152">
-        <v>0</v>
-      </c>
+      <c r="C22" s="150"/>
+      <c r="D22" s="152"/>
+      <c r="E22" s="152"/>
+      <c r="F22" s="154"/>
+      <c r="G22" s="152"/>
+      <c r="H22" s="152"/>
+      <c r="I22" s="152"/>
+      <c r="J22" s="152"/>
       <c r="N22" s="143"/>
       <c r="O22" s="143"/>
     </row>
     <row r="23" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="150">
-        <v>39155</v>
-      </c>
-      <c r="D23" s="152">
-        <v>13.2</v>
-      </c>
-      <c r="E23" s="152">
-        <v>332.4</v>
-      </c>
-      <c r="F23" s="154">
-        <v>7.76</v>
-      </c>
-      <c r="G23" s="152">
-        <v>4.8</v>
-      </c>
-      <c r="H23" s="152">
-        <v>2.4</v>
-      </c>
-      <c r="I23" s="152">
-        <v>4.5</v>
-      </c>
-      <c r="J23" s="152">
-        <v>0.2</v>
-      </c>
+      <c r="C23" s="150"/>
+      <c r="D23" s="152"/>
+      <c r="E23" s="152"/>
+      <c r="F23" s="154"/>
+      <c r="G23" s="152"/>
+      <c r="H23" s="152"/>
+      <c r="I23" s="152"/>
+      <c r="J23" s="152"/>
       <c r="N23" s="143"/>
       <c r="O23" s="143"/>
     </row>
     <row r="24" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="150">
-        <v>38777</v>
-      </c>
-      <c r="D24" s="152">
-        <v>15.2</v>
-      </c>
-      <c r="E24" s="152">
-        <v>355.7</v>
-      </c>
-      <c r="F24" s="154">
-        <v>7.78</v>
-      </c>
-      <c r="G24" s="152">
-        <v>5.7</v>
-      </c>
-      <c r="H24" s="152">
-        <v>4.3</v>
-      </c>
-      <c r="I24" s="152">
-        <v>4.8</v>
-      </c>
-      <c r="J24" s="152">
-        <v>0.4</v>
-      </c>
+      <c r="C24" s="150"/>
+      <c r="D24" s="152"/>
+      <c r="E24" s="152"/>
+      <c r="F24" s="154"/>
+      <c r="G24" s="152"/>
+      <c r="H24" s="152"/>
+      <c r="I24" s="152"/>
+      <c r="J24" s="152"/>
       <c r="N24" s="143"/>
       <c r="O24" s="143"/>
     </row>
     <row r="25" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="150">
-        <v>38414</v>
-      </c>
-      <c r="D25" s="152">
-        <v>12.8</v>
-      </c>
-      <c r="E25" s="152">
-        <v>380.6</v>
-      </c>
-      <c r="F25" s="154">
-        <v>7.47</v>
-      </c>
-      <c r="G25" s="152">
-        <v>5.9</v>
-      </c>
-      <c r="H25" s="152">
-        <v>0</v>
-      </c>
-      <c r="I25" s="152">
-        <v>4.8</v>
-      </c>
-      <c r="J25" s="152">
-        <v>0</v>
-      </c>
+      <c r="C25" s="150"/>
+      <c r="D25" s="152"/>
+      <c r="E25" s="152"/>
+      <c r="F25" s="154"/>
+      <c r="G25" s="152"/>
+      <c r="H25" s="152"/>
+      <c r="I25" s="152"/>
+      <c r="J25" s="152"/>
       <c r="N25" s="143"/>
       <c r="O25" s="143"/>
     </row>
     <row r="26" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="150">
-        <v>38015</v>
-      </c>
-      <c r="D26" s="152">
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="E26" s="152">
-        <v>345.4</v>
-      </c>
-      <c r="F26" s="154">
-        <v>6.86</v>
-      </c>
-      <c r="G26" s="152">
-        <v>4.9000000000000004</v>
-      </c>
-      <c r="H26" s="152">
-        <v>0</v>
-      </c>
-      <c r="I26" s="152">
-        <v>4.2</v>
-      </c>
-      <c r="J26" s="152">
-        <v>0</v>
-      </c>
+      <c r="C26" s="150"/>
+      <c r="D26" s="152"/>
+      <c r="E26" s="152"/>
+      <c r="F26" s="154"/>
+      <c r="G26" s="152"/>
+      <c r="H26" s="152"/>
+      <c r="I26" s="152"/>
+      <c r="J26" s="152"/>
       <c r="N26" s="143"/>
       <c r="O26" s="143"/>
     </row>
     <row r="27" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="150">
-        <v>37649</v>
-      </c>
-      <c r="D27" s="152">
-        <v>11.6</v>
-      </c>
-      <c r="E27" s="152">
-        <v>433.6</v>
-      </c>
-      <c r="F27" s="154">
-        <v>6.34</v>
-      </c>
-      <c r="G27" s="152">
-        <v>7</v>
-      </c>
-      <c r="H27" s="152">
-        <v>1.4</v>
-      </c>
-      <c r="I27" s="152">
-        <v>5.2</v>
-      </c>
-      <c r="J27" s="152">
-        <v>0</v>
-      </c>
+      <c r="C27" s="150"/>
+      <c r="D27" s="152"/>
+      <c r="E27" s="152"/>
+      <c r="F27" s="154"/>
+      <c r="G27" s="152"/>
+      <c r="H27" s="152"/>
+      <c r="I27" s="152"/>
+      <c r="J27" s="152"/>
       <c r="N27" s="143"/>
       <c r="O27" s="143"/>
     </row>
     <row r="28" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="150">
-        <v>37321</v>
-      </c>
-      <c r="D28" s="152">
-        <v>10.1</v>
-      </c>
-      <c r="E28" s="152">
-        <v>380.5</v>
-      </c>
-      <c r="F28" s="154">
-        <v>7.3</v>
-      </c>
-      <c r="G28" s="152">
-        <v>6.8</v>
-      </c>
-      <c r="H28" s="152">
-        <v>2.9</v>
-      </c>
-      <c r="I28" s="152">
-        <v>6.2</v>
-      </c>
-      <c r="J28" s="152">
-        <v>1.8</v>
-      </c>
+      <c r="C28" s="150"/>
+      <c r="D28" s="152"/>
+      <c r="E28" s="152"/>
+      <c r="F28" s="154"/>
+      <c r="G28" s="152"/>
+      <c r="H28" s="152"/>
+      <c r="I28" s="152"/>
+      <c r="J28" s="152"/>
       <c r="N28" s="143"/>
       <c r="O28" s="143"/>
     </row>
     <row r="29" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="150">
-        <v>37062</v>
-      </c>
-      <c r="D29" s="152">
-        <v>15</v>
-      </c>
-      <c r="E29" s="152">
-        <v>251</v>
-      </c>
-      <c r="F29" s="154">
-        <v>4.9400000000000004</v>
-      </c>
-      <c r="G29" s="152">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="H29" s="152">
-        <v>0</v>
-      </c>
-      <c r="I29" s="152">
-        <v>4.3</v>
-      </c>
-      <c r="J29" s="152">
-        <v>1.4</v>
-      </c>
+      <c r="C29" s="150"/>
+      <c r="D29" s="152"/>
+      <c r="E29" s="152"/>
+      <c r="F29" s="154"/>
+      <c r="G29" s="152"/>
+      <c r="H29" s="152"/>
+      <c r="I29" s="152"/>
+      <c r="J29" s="152"/>
       <c r="N29" s="143"/>
       <c r="O29" s="143"/>
     </row>
     <row r="30" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="150">
-        <v>36684</v>
-      </c>
-      <c r="D30" s="152">
-        <v>17</v>
-      </c>
-      <c r="E30" s="152">
-        <v>357</v>
-      </c>
-      <c r="F30" s="154">
-        <v>7.38</v>
-      </c>
-      <c r="G30" s="152">
-        <v>5.6</v>
-      </c>
-      <c r="H30" s="152">
-        <v>1.3</v>
-      </c>
-      <c r="I30" s="152">
-        <v>6.3</v>
-      </c>
-      <c r="J30" s="152">
-        <v>0</v>
-      </c>
+      <c r="C30" s="150"/>
+      <c r="D30" s="152"/>
+      <c r="E30" s="152"/>
+      <c r="F30" s="154"/>
+      <c r="G30" s="152"/>
+      <c r="H30" s="152"/>
+      <c r="I30" s="152"/>
+      <c r="J30" s="152"/>
       <c r="N30" s="143"/>
       <c r="O30" s="143"/>
     </row>
     <row r="31" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="150">
-        <v>36166</v>
-      </c>
-      <c r="D31" s="152">
-        <v>8.4</v>
-      </c>
-      <c r="E31" s="152">
-        <v>280.7</v>
-      </c>
-      <c r="F31" s="154">
-        <v>5.61</v>
-      </c>
-      <c r="G31" s="152">
-        <v>5.4</v>
-      </c>
-      <c r="H31" s="152">
-        <v>1.9</v>
-      </c>
-      <c r="I31" s="152">
-        <v>6.5</v>
-      </c>
-      <c r="J31" s="152">
-        <v>0</v>
-      </c>
+      <c r="C31" s="150"/>
+      <c r="D31" s="152"/>
+      <c r="E31" s="152"/>
+      <c r="F31" s="154"/>
+      <c r="G31" s="152"/>
+      <c r="H31" s="152"/>
+      <c r="I31" s="152"/>
+      <c r="J31" s="152"/>
       <c r="N31" s="143"/>
       <c r="O31" s="143"/>
     </row>
     <row r="32" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="150">
-        <v>35838</v>
-      </c>
-      <c r="D32" s="152">
-        <v>12</v>
-      </c>
-      <c r="E32" s="152">
-        <v>372</v>
-      </c>
-      <c r="F32" s="154">
-        <v>6</v>
-      </c>
-      <c r="G32" s="152">
-        <v>8</v>
-      </c>
-      <c r="H32" s="152">
-        <v>2</v>
-      </c>
-      <c r="I32" s="152">
-        <v>9</v>
-      </c>
-      <c r="J32" s="152">
-        <v>0</v>
-      </c>
+      <c r="C32" s="150"/>
+      <c r="D32" s="152"/>
+      <c r="E32" s="152"/>
+      <c r="F32" s="154"/>
+      <c r="G32" s="152"/>
+      <c r="H32" s="152"/>
+      <c r="I32" s="152"/>
+      <c r="J32" s="152"/>
       <c r="N32" s="143"/>
       <c r="O32" s="143"/>
     </row>
     <row r="33" spans="3:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="150">
-        <v>35460</v>
-      </c>
-      <c r="D33" s="152">
-        <v>7</v>
-      </c>
-      <c r="E33" s="152">
-        <v>240</v>
-      </c>
-      <c r="F33" s="154">
-        <v>3.5</v>
-      </c>
-      <c r="G33" s="152">
-        <v>5</v>
-      </c>
-      <c r="H33" s="152">
-        <v>1</v>
-      </c>
-      <c r="I33" s="152">
-        <v>4</v>
-      </c>
-      <c r="J33" s="152">
-        <v>0</v>
-      </c>
+      <c r="C33" s="150"/>
+      <c r="D33" s="152"/>
+      <c r="E33" s="152"/>
+      <c r="F33" s="154"/>
+      <c r="G33" s="152"/>
+      <c r="H33" s="152"/>
+      <c r="I33" s="152"/>
+      <c r="J33" s="152"/>
       <c r="N33" s="143"/>
       <c r="O33" s="143"/>
     </row>
     <row r="34" spans="3:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="150">
-        <v>34374</v>
-      </c>
-      <c r="D34" s="152">
-        <v>11</v>
-      </c>
-      <c r="E34" s="152">
-        <v>94</v>
-      </c>
-      <c r="F34" s="154" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G34" s="152">
-        <v>1</v>
-      </c>
-      <c r="H34" s="152">
-        <v>1</v>
-      </c>
-      <c r="I34" s="152">
-        <v>1</v>
-      </c>
-      <c r="J34" s="152">
-        <v>0</v>
-      </c>
+      <c r="C34" s="150"/>
+      <c r="D34" s="152"/>
+      <c r="E34" s="152"/>
+      <c r="F34" s="154"/>
+      <c r="G34" s="152"/>
+      <c r="H34" s="152"/>
+      <c r="I34" s="152"/>
+      <c r="J34" s="152"/>
     </row>
     <row r="35" spans="3:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="150">
-        <v>34303</v>
-      </c>
-      <c r="D35" s="152">
-        <v>4</v>
-      </c>
-      <c r="E35" s="152">
-        <v>4</v>
-      </c>
-      <c r="F35" s="154" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="G35" s="152">
-        <v>1</v>
-      </c>
-      <c r="H35" s="152">
-        <v>0</v>
-      </c>
-      <c r="I35" s="152">
-        <v>1</v>
-      </c>
-      <c r="J35" s="152">
-        <v>0</v>
-      </c>
+      <c r="C35" s="150"/>
+      <c r="D35" s="152"/>
+      <c r="E35" s="152"/>
+      <c r="F35" s="154"/>
+      <c r="G35" s="152"/>
+      <c r="H35" s="152"/>
+      <c r="I35" s="152"/>
+      <c r="J35" s="152"/>
       <c r="V35" s="149"/>
       <c r="W35" s="149"/>
       <c r="X35" s="149"/>
@@ -8926,7 +8580,7 @@
         <v>82</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="S2" s="96">
         <f>'2-FAL'!A4</f>
@@ -9043,7 +8697,7 @@
         <v>81</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="S5" s="96">
         <f>'2-FAL'!A7</f>
@@ -9085,7 +8739,7 @@
         <v>81</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="S6" s="96">
         <f>'2-FAL'!A8</f>
@@ -9131,7 +8785,7 @@
         <v>81</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="S7" s="96">
         <f>'2-FAL'!A9</f>
@@ -9243,7 +8897,7 @@
         <v>78</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="S9" s="96">
         <f>'2-FAL'!A11</f>
@@ -16069,6 +15723,44 @@
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="T47:T53"/>
+    <mergeCell ref="T62:T68"/>
+    <mergeCell ref="I77:I83"/>
+    <mergeCell ref="A73:I74"/>
+    <mergeCell ref="L58:T59"/>
+    <mergeCell ref="T2:T8"/>
+    <mergeCell ref="T17:T23"/>
+    <mergeCell ref="T32:T38"/>
+    <mergeCell ref="L43:T44"/>
+    <mergeCell ref="L28:T29"/>
+    <mergeCell ref="L13:T14"/>
+    <mergeCell ref="I2:I8"/>
+    <mergeCell ref="A13:I14"/>
+    <mergeCell ref="I17:I23"/>
+    <mergeCell ref="A28:I29"/>
+    <mergeCell ref="I32:I38"/>
+    <mergeCell ref="A43:I44"/>
+    <mergeCell ref="I47:I53"/>
+    <mergeCell ref="A58:I59"/>
+    <mergeCell ref="I62:I68"/>
+    <mergeCell ref="A103:I104"/>
+    <mergeCell ref="A88:I89"/>
+    <mergeCell ref="I92:I98"/>
+    <mergeCell ref="I107:I113"/>
+    <mergeCell ref="A118:I119"/>
+    <mergeCell ref="I122:I128"/>
+    <mergeCell ref="A133:I134"/>
+    <mergeCell ref="I137:I143"/>
+    <mergeCell ref="A148:I149"/>
+    <mergeCell ref="I152:I158"/>
+    <mergeCell ref="A163:I164"/>
+    <mergeCell ref="I167:I173"/>
+    <mergeCell ref="A178:I179"/>
+    <mergeCell ref="I182:I188"/>
+    <mergeCell ref="A193:I194"/>
+    <mergeCell ref="I197:I203"/>
+    <mergeCell ref="A208:I209"/>
+    <mergeCell ref="I212:I218"/>
     <mergeCell ref="I257:I263"/>
     <mergeCell ref="A268:I269"/>
     <mergeCell ref="I272:I278"/>
@@ -16077,44 +15769,6 @@
     <mergeCell ref="A238:I239"/>
     <mergeCell ref="I242:I248"/>
     <mergeCell ref="A253:I254"/>
-    <mergeCell ref="I182:I188"/>
-    <mergeCell ref="A193:I194"/>
-    <mergeCell ref="I197:I203"/>
-    <mergeCell ref="A208:I209"/>
-    <mergeCell ref="I212:I218"/>
-    <mergeCell ref="A148:I149"/>
-    <mergeCell ref="I152:I158"/>
-    <mergeCell ref="A163:I164"/>
-    <mergeCell ref="I167:I173"/>
-    <mergeCell ref="A178:I179"/>
-    <mergeCell ref="I107:I113"/>
-    <mergeCell ref="A118:I119"/>
-    <mergeCell ref="I122:I128"/>
-    <mergeCell ref="A133:I134"/>
-    <mergeCell ref="I137:I143"/>
-    <mergeCell ref="A43:I44"/>
-    <mergeCell ref="I47:I53"/>
-    <mergeCell ref="A58:I59"/>
-    <mergeCell ref="I62:I68"/>
-    <mergeCell ref="A103:I104"/>
-    <mergeCell ref="A88:I89"/>
-    <mergeCell ref="I92:I98"/>
-    <mergeCell ref="I2:I8"/>
-    <mergeCell ref="A13:I14"/>
-    <mergeCell ref="I17:I23"/>
-    <mergeCell ref="A28:I29"/>
-    <mergeCell ref="I32:I38"/>
-    <mergeCell ref="T2:T8"/>
-    <mergeCell ref="T17:T23"/>
-    <mergeCell ref="T32:T38"/>
-    <mergeCell ref="L43:T44"/>
-    <mergeCell ref="L28:T29"/>
-    <mergeCell ref="L13:T14"/>
-    <mergeCell ref="T47:T53"/>
-    <mergeCell ref="T62:T68"/>
-    <mergeCell ref="I77:I83"/>
-    <mergeCell ref="A73:I74"/>
-    <mergeCell ref="L58:T59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17249,7 +16903,7 @@
         <v>#REF!</v>
       </c>
       <c r="H1" s="20"/>
-      <c r="I1" s="184" t="e">
+      <c r="I1" s="204" t="e">
         <f>GOT!#REF!</f>
         <v>#REF!</v>
       </c>
@@ -17282,7 +16936,7 @@
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
-      <c r="I2" s="185"/>
+      <c r="I2" s="205"/>
       <c r="L2" s="55"/>
       <c r="M2" s="30" t="s">
         <v>112</v>
@@ -17302,7 +16956,7 @@
         <v>1.6666666666666667</v>
       </c>
       <c r="S2" s="20"/>
-      <c r="T2" s="184">
+      <c r="T2" s="204">
         <f>GOT!F3</f>
         <v>39547</v>
       </c>
@@ -17312,10 +16966,10 @@
       <c r="AZ2" s="87">
         <v>72.5</v>
       </c>
-      <c r="BA2" s="189" t="s">
+      <c r="BA2" s="197" t="s">
         <v>112</v>
       </c>
-      <c r="BB2" s="191" t="s">
+      <c r="BB2" s="199" t="s">
         <v>113</v>
       </c>
     </row>
@@ -17338,7 +16992,7 @@
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20"/>
-      <c r="I3" s="185"/>
+      <c r="I3" s="205"/>
       <c r="L3" s="58" t="s">
         <v>119</v>
       </c>
@@ -17357,11 +17011,11 @@
       <c r="Q3" s="20"/>
       <c r="R3" s="20"/>
       <c r="S3" s="20"/>
-      <c r="T3" s="185"/>
+      <c r="T3" s="205"/>
       <c r="AY3" s="88"/>
       <c r="AZ3" s="89"/>
-      <c r="BA3" s="190"/>
-      <c r="BB3" s="192"/>
+      <c r="BA3" s="198"/>
+      <c r="BB3" s="200"/>
     </row>
     <row r="4" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="63" t="s">
@@ -17382,7 +17036,7 @@
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
-      <c r="I4" s="185"/>
+      <c r="I4" s="205"/>
       <c r="L4" s="61" t="s">
         <v>114</v>
       </c>
@@ -17401,8 +17055,8 @@
       <c r="Q4" s="20"/>
       <c r="R4" s="20"/>
       <c r="S4" s="20"/>
-      <c r="T4" s="185"/>
-      <c r="AY4" s="193" t="s">
+      <c r="T4" s="205"/>
+      <c r="AY4" s="194" t="s">
         <v>133</v>
       </c>
       <c r="AZ4" s="90" t="s">
@@ -17411,7 +17065,7 @@
       <c r="BA4" s="59">
         <v>1</v>
       </c>
-      <c r="BB4" s="196">
+      <c r="BB4" s="187">
         <v>3</v>
       </c>
     </row>
@@ -17439,7 +17093,7 @@
         <v>#REF!</v>
       </c>
       <c r="H5" s="20"/>
-      <c r="I5" s="185"/>
+      <c r="I5" s="205"/>
       <c r="L5" s="63" t="s">
         <v>116</v>
       </c>
@@ -17458,15 +17112,15 @@
       <c r="Q5" s="20"/>
       <c r="R5" s="20"/>
       <c r="S5" s="20"/>
-      <c r="T5" s="185"/>
-      <c r="AY5" s="194"/>
+      <c r="T5" s="205"/>
+      <c r="AY5" s="195"/>
       <c r="AZ5" s="59">
         <v>50</v>
       </c>
       <c r="BA5" s="59">
         <v>2</v>
       </c>
-      <c r="BB5" s="196"/>
+      <c r="BB5" s="187"/>
     </row>
     <row r="6" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="66" t="s">
@@ -17511,15 +17165,15 @@
         <v>2</v>
       </c>
       <c r="S6" s="20"/>
-      <c r="T6" s="185"/>
-      <c r="AY6" s="194"/>
+      <c r="T6" s="205"/>
+      <c r="AY6" s="195"/>
       <c r="AZ6" s="59">
         <v>40</v>
       </c>
       <c r="BA6" s="59">
         <v>3</v>
       </c>
-      <c r="BB6" s="196"/>
+      <c r="BB6" s="187"/>
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
@@ -17550,25 +17204,25 @@
       <c r="R7" s="67"/>
       <c r="S7" s="20"/>
       <c r="T7" s="20"/>
-      <c r="AY7" s="195"/>
+      <c r="AY7" s="196"/>
       <c r="AZ7" s="59">
         <v>30</v>
       </c>
       <c r="BA7" s="59">
         <v>4</v>
       </c>
-      <c r="BB7" s="196"/>
+      <c r="BB7" s="187"/>
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A8" s="186"/>
-      <c r="B8" s="186"/>
-      <c r="C8" s="186"/>
-      <c r="D8" s="186"/>
-      <c r="E8" s="186"/>
-      <c r="F8" s="186"/>
-      <c r="G8" s="186"/>
-      <c r="H8" s="186"/>
-      <c r="I8" s="186"/>
+      <c r="A8" s="184"/>
+      <c r="B8" s="184"/>
+      <c r="C8" s="184"/>
+      <c r="D8" s="184"/>
+      <c r="E8" s="184"/>
+      <c r="F8" s="184"/>
+      <c r="G8" s="184"/>
+      <c r="H8" s="184"/>
+      <c r="I8" s="184"/>
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
       <c r="N8" s="20"/>
@@ -17578,7 +17232,7 @@
       <c r="R8" s="20"/>
       <c r="S8" s="20"/>
       <c r="T8" s="20"/>
-      <c r="AY8" s="197" t="s">
+      <c r="AY8" s="201" t="s">
         <v>114</v>
       </c>
       <c r="AZ8" s="91">
@@ -17587,56 +17241,56 @@
       <c r="BA8" s="59">
         <v>1</v>
       </c>
-      <c r="BB8" s="196">
+      <c r="BB8" s="187">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A9" s="186"/>
-      <c r="B9" s="186"/>
-      <c r="C9" s="186"/>
-      <c r="D9" s="186"/>
-      <c r="E9" s="186"/>
-      <c r="F9" s="186"/>
-      <c r="G9" s="186"/>
-      <c r="H9" s="186"/>
-      <c r="I9" s="186"/>
-      <c r="L9" s="186"/>
-      <c r="M9" s="186"/>
-      <c r="N9" s="186"/>
-      <c r="O9" s="186"/>
-      <c r="P9" s="186"/>
-      <c r="Q9" s="186"/>
-      <c r="R9" s="186"/>
-      <c r="S9" s="186"/>
-      <c r="T9" s="186"/>
-      <c r="AY9" s="198"/>
+      <c r="A9" s="184"/>
+      <c r="B9" s="184"/>
+      <c r="C9" s="184"/>
+      <c r="D9" s="184"/>
+      <c r="E9" s="184"/>
+      <c r="F9" s="184"/>
+      <c r="G9" s="184"/>
+      <c r="H9" s="184"/>
+      <c r="I9" s="184"/>
+      <c r="L9" s="184"/>
+      <c r="M9" s="184"/>
+      <c r="N9" s="184"/>
+      <c r="O9" s="184"/>
+      <c r="P9" s="184"/>
+      <c r="Q9" s="184"/>
+      <c r="R9" s="184"/>
+      <c r="S9" s="184"/>
+      <c r="T9" s="184"/>
+      <c r="AY9" s="202"/>
       <c r="AZ9" s="59">
         <v>30</v>
       </c>
       <c r="BA9" s="59">
         <v>2</v>
       </c>
-      <c r="BB9" s="196"/>
+      <c r="BB9" s="187"/>
     </row>
     <row r="10" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="L10" s="186"/>
-      <c r="M10" s="186"/>
-      <c r="N10" s="186"/>
-      <c r="O10" s="186"/>
-      <c r="P10" s="186"/>
-      <c r="Q10" s="186"/>
-      <c r="R10" s="186"/>
-      <c r="S10" s="186"/>
-      <c r="T10" s="186"/>
-      <c r="AY10" s="198"/>
+      <c r="L10" s="184"/>
+      <c r="M10" s="184"/>
+      <c r="N10" s="184"/>
+      <c r="O10" s="184"/>
+      <c r="P10" s="184"/>
+      <c r="Q10" s="184"/>
+      <c r="R10" s="184"/>
+      <c r="S10" s="184"/>
+      <c r="T10" s="184"/>
+      <c r="AY10" s="202"/>
       <c r="AZ10" s="59">
         <v>40</v>
       </c>
       <c r="BA10" s="59">
         <v>3</v>
       </c>
-      <c r="BB10" s="196"/>
+      <c r="BB10" s="187"/>
     </row>
     <row r="11" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A11" s="55"/>
@@ -17657,20 +17311,20 @@
         <f>SUM(D12:D16)/(SUM(C12:C16))</f>
         <v>#REF!</v>
       </c>
-      <c r="I11" s="187" t="e">
+      <c r="I11" s="185" t="e">
         <f>GOT!#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="AQ11" s="36"/>
       <c r="AR11" s="36"/>
-      <c r="AY11" s="199"/>
+      <c r="AY11" s="203"/>
       <c r="AZ11" s="90" t="s">
         <v>135</v>
       </c>
       <c r="BA11" s="59">
         <v>4</v>
       </c>
-      <c r="BB11" s="196"/>
+      <c r="BB11" s="187"/>
     </row>
     <row r="12" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
@@ -17690,7 +17344,7 @@
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
-      <c r="I12" s="188"/>
+      <c r="I12" s="186"/>
       <c r="L12" s="55"/>
       <c r="M12" s="30" t="s">
         <v>112</v>
@@ -17709,13 +17363,13 @@
         <f>SUM(O13:O17)/(SUM(N13:N17))</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="T12" s="187">
+      <c r="T12" s="185">
         <f>GOT!E3</f>
         <v>39850</v>
       </c>
       <c r="AQ12" s="36"/>
       <c r="AR12" s="36"/>
-      <c r="AY12" s="193" t="s">
+      <c r="AY12" s="194" t="s">
         <v>136</v>
       </c>
       <c r="AZ12" s="59">
@@ -17724,7 +17378,7 @@
       <c r="BA12" s="59">
         <v>1</v>
       </c>
-      <c r="BB12" s="196">
+      <c r="BB12" s="187">
         <v>1</v>
       </c>
     </row>
@@ -17746,7 +17400,7 @@
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
-      <c r="I13" s="188"/>
+      <c r="I13" s="186"/>
       <c r="L13" s="58" t="s">
         <v>119</v>
       </c>
@@ -17764,17 +17418,17 @@
       <c r="P13" s="20"/>
       <c r="Q13" s="20"/>
       <c r="R13" s="20"/>
-      <c r="T13" s="188"/>
+      <c r="T13" s="186"/>
       <c r="AQ13" s="36"/>
       <c r="AR13" s="36"/>
-      <c r="AY13" s="194"/>
+      <c r="AY13" s="195"/>
       <c r="AZ13" s="59">
         <v>0.1</v>
       </c>
       <c r="BA13" s="59">
         <v>2</v>
       </c>
-      <c r="BB13" s="196"/>
+      <c r="BB13" s="187"/>
     </row>
     <row r="14" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="63" t="s">
@@ -17794,7 +17448,7 @@
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
-      <c r="I14" s="188"/>
+      <c r="I14" s="186"/>
       <c r="L14" s="61" t="s">
         <v>114</v>
       </c>
@@ -17812,17 +17466,17 @@
       <c r="P14" s="20"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="20"/>
-      <c r="T14" s="188"/>
+      <c r="T14" s="186"/>
       <c r="AQ14" s="69"/>
       <c r="AR14" s="69"/>
-      <c r="AY14" s="194"/>
+      <c r="AY14" s="195"/>
       <c r="AZ14" s="59">
         <v>0.2</v>
       </c>
       <c r="BA14" s="59">
         <v>3</v>
       </c>
-      <c r="BB14" s="196"/>
+      <c r="BB14" s="187"/>
     </row>
     <row r="15" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="61" t="s">
@@ -17848,7 +17502,7 @@
         <v>#REF!</v>
       </c>
       <c r="H15" s="20"/>
-      <c r="I15" s="188"/>
+      <c r="I15" s="186"/>
       <c r="L15" s="63" t="s">
         <v>116</v>
       </c>
@@ -17866,17 +17520,17 @@
       <c r="P15" s="20"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="20"/>
-      <c r="T15" s="188"/>
+      <c r="T15" s="186"/>
       <c r="AQ15" s="69"/>
       <c r="AR15" s="69"/>
-      <c r="AY15" s="195"/>
+      <c r="AY15" s="196"/>
       <c r="AZ15" s="90" t="s">
         <v>137</v>
       </c>
       <c r="BA15" s="59">
         <v>4</v>
       </c>
-      <c r="BB15" s="196"/>
+      <c r="BB15" s="187"/>
     </row>
     <row r="16" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="66" t="s">
@@ -17920,10 +17574,10 @@
         <v>2</v>
       </c>
       <c r="S16" s="20"/>
-      <c r="T16" s="188"/>
+      <c r="T16" s="186"/>
       <c r="AQ16" s="45"/>
       <c r="AR16" s="69"/>
-      <c r="AY16" s="200" t="s">
+      <c r="AY16" s="188" t="s">
         <v>110</v>
       </c>
       <c r="AZ16" s="59">
@@ -17932,7 +17586,7 @@
       <c r="BA16" s="59">
         <v>1</v>
       </c>
-      <c r="BB16" s="203">
+      <c r="BB16" s="191">
         <v>2</v>
       </c>
     </row>
@@ -17955,76 +17609,76 @@
       <c r="Q17" s="67"/>
       <c r="R17" s="67"/>
       <c r="S17" s="20"/>
-      <c r="AY17" s="201"/>
+      <c r="AY17" s="189"/>
       <c r="AZ17" s="59">
         <v>2</v>
       </c>
       <c r="BA17" s="59">
         <v>2</v>
       </c>
-      <c r="BB17" s="204"/>
+      <c r="BB17" s="192"/>
     </row>
     <row r="18" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A18" s="186"/>
-      <c r="B18" s="186"/>
-      <c r="C18" s="186"/>
-      <c r="D18" s="186"/>
-      <c r="E18" s="186"/>
-      <c r="F18" s="186"/>
-      <c r="G18" s="186"/>
-      <c r="H18" s="186"/>
-      <c r="I18" s="186"/>
+      <c r="A18" s="184"/>
+      <c r="B18" s="184"/>
+      <c r="C18" s="184"/>
+      <c r="D18" s="184"/>
+      <c r="E18" s="184"/>
+      <c r="F18" s="184"/>
+      <c r="G18" s="184"/>
+      <c r="H18" s="184"/>
+      <c r="I18" s="184"/>
       <c r="S18" s="20"/>
-      <c r="AY18" s="201"/>
+      <c r="AY18" s="189"/>
       <c r="AZ18" s="59">
         <v>2.5</v>
       </c>
       <c r="BA18" s="59">
         <v>3</v>
       </c>
-      <c r="BB18" s="204"/>
+      <c r="BB18" s="192"/>
     </row>
     <row r="19" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A19" s="186"/>
-      <c r="B19" s="186"/>
-      <c r="C19" s="186"/>
-      <c r="D19" s="186"/>
-      <c r="E19" s="186"/>
-      <c r="F19" s="186"/>
-      <c r="G19" s="186"/>
-      <c r="H19" s="186"/>
-      <c r="I19" s="186"/>
-      <c r="L19" s="186"/>
-      <c r="M19" s="186"/>
-      <c r="N19" s="186"/>
-      <c r="O19" s="186"/>
-      <c r="P19" s="186"/>
-      <c r="Q19" s="186"/>
-      <c r="R19" s="186"/>
-      <c r="S19" s="186"/>
-      <c r="T19" s="186"/>
+      <c r="A19" s="184"/>
+      <c r="B19" s="184"/>
+      <c r="C19" s="184"/>
+      <c r="D19" s="184"/>
+      <c r="E19" s="184"/>
+      <c r="F19" s="184"/>
+      <c r="G19" s="184"/>
+      <c r="H19" s="184"/>
+      <c r="I19" s="184"/>
+      <c r="L19" s="184"/>
+      <c r="M19" s="184"/>
+      <c r="N19" s="184"/>
+      <c r="O19" s="184"/>
+      <c r="P19" s="184"/>
+      <c r="Q19" s="184"/>
+      <c r="R19" s="184"/>
+      <c r="S19" s="184"/>
+      <c r="T19" s="184"/>
       <c r="AQ19" s="20"/>
       <c r="AR19" s="20"/>
-      <c r="AY19" s="202"/>
+      <c r="AY19" s="190"/>
       <c r="AZ19" s="59" t="s">
         <v>138</v>
       </c>
       <c r="BA19" s="59">
         <v>4</v>
       </c>
-      <c r="BB19" s="205"/>
+      <c r="BB19" s="193"/>
     </row>
     <row r="20" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="L20" s="186"/>
-      <c r="M20" s="186"/>
-      <c r="N20" s="186"/>
-      <c r="O20" s="186"/>
-      <c r="P20" s="186"/>
-      <c r="Q20" s="186"/>
-      <c r="R20" s="186"/>
-      <c r="S20" s="186"/>
-      <c r="T20" s="186"/>
-      <c r="AY20" s="193" t="s">
+      <c r="L20" s="184"/>
+      <c r="M20" s="184"/>
+      <c r="N20" s="184"/>
+      <c r="O20" s="184"/>
+      <c r="P20" s="184"/>
+      <c r="Q20" s="184"/>
+      <c r="R20" s="184"/>
+      <c r="S20" s="184"/>
+      <c r="T20" s="184"/>
+      <c r="AY20" s="194" t="s">
         <v>139</v>
       </c>
       <c r="AZ20" s="90" t="s">
@@ -18033,7 +17687,7 @@
       <c r="BA20" s="59">
         <v>1</v>
       </c>
-      <c r="BB20" s="196">
+      <c r="BB20" s="187">
         <v>2</v>
       </c>
     </row>
@@ -18056,18 +17710,18 @@
         <f>SUM(D22:D26)/(SUM(C22:C26))</f>
         <v>#REF!</v>
       </c>
-      <c r="I21" s="187" t="e">
+      <c r="I21" s="185" t="e">
         <f>GOT!#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="AY21" s="194"/>
+      <c r="AY21" s="195"/>
       <c r="AZ21" s="91">
         <v>35</v>
       </c>
       <c r="BA21" s="59">
         <v>2</v>
       </c>
-      <c r="BB21" s="196"/>
+      <c r="BB21" s="187"/>
     </row>
     <row r="22" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
@@ -18087,7 +17741,7 @@
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
-      <c r="I22" s="188"/>
+      <c r="I22" s="186"/>
       <c r="L22" s="55"/>
       <c r="M22" s="30" t="s">
         <v>112</v>
@@ -18106,7 +17760,7 @@
         <f>SUM(O23:O27)/(SUM(N23:N27))</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="T22" s="187">
+      <c r="T22" s="185">
         <f>GOT!D3</f>
         <v>40254</v>
       </c>
@@ -18119,14 +17773,14 @@
       <c r="AU22" s="1">
         <v>2010</v>
       </c>
-      <c r="AY22" s="194"/>
+      <c r="AY22" s="195"/>
       <c r="AZ22" s="91">
         <v>30</v>
       </c>
       <c r="BA22" s="59">
         <v>3</v>
       </c>
-      <c r="BB22" s="196"/>
+      <c r="BB22" s="187"/>
     </row>
     <row r="23" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A23" s="61" t="s">
@@ -18146,7 +17800,7 @@
       <c r="E23" s="20"/>
       <c r="F23" s="20"/>
       <c r="G23" s="20"/>
-      <c r="I23" s="188"/>
+      <c r="I23" s="186"/>
       <c r="L23" s="58" t="s">
         <v>119</v>
       </c>
@@ -18164,7 +17818,7 @@
       <c r="P23" s="20"/>
       <c r="Q23" s="20"/>
       <c r="R23" s="20"/>
-      <c r="T23" s="188"/>
+      <c r="T23" s="186"/>
       <c r="AQ23" s="20"/>
       <c r="AR23" s="20"/>
       <c r="AT23" s="112">
@@ -18174,14 +17828,14 @@
       <c r="AU23" s="1">
         <v>2012</v>
       </c>
-      <c r="AY23" s="195"/>
+      <c r="AY23" s="196"/>
       <c r="AZ23" s="91">
         <v>25</v>
       </c>
       <c r="BA23" s="59">
         <v>4</v>
       </c>
-      <c r="BB23" s="196"/>
+      <c r="BB23" s="187"/>
     </row>
     <row r="24" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="63" t="s">
@@ -18201,7 +17855,7 @@
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
-      <c r="I24" s="188"/>
+      <c r="I24" s="186"/>
       <c r="L24" s="61" t="s">
         <v>114</v>
       </c>
@@ -18219,7 +17873,7 @@
       <c r="P24" s="20"/>
       <c r="Q24" s="20"/>
       <c r="R24" s="20"/>
-      <c r="T24" s="188"/>
+      <c r="T24" s="186"/>
       <c r="AQ24" s="20"/>
       <c r="AR24" s="20"/>
       <c r="AT24" s="112">
@@ -18254,7 +17908,7 @@
         <v>#REF!</v>
       </c>
       <c r="H25" s="20"/>
-      <c r="I25" s="188"/>
+      <c r="I25" s="186"/>
       <c r="L25" s="63" t="s">
         <v>116</v>
       </c>
@@ -18272,7 +17926,7 @@
       <c r="P25" s="20"/>
       <c r="Q25" s="20"/>
       <c r="R25" s="20"/>
-      <c r="T25" s="188"/>
+      <c r="T25" s="186"/>
       <c r="AT25" s="112">
         <f>$R$32</f>
         <v>1.9166666666666667</v>
@@ -18323,7 +17977,7 @@
         <v>2</v>
       </c>
       <c r="S26" s="20"/>
-      <c r="T26" s="188"/>
+      <c r="T26" s="186"/>
       <c r="AT26" s="112">
         <f>R42</f>
         <v>1.9166666666666667</v>
@@ -18354,47 +18008,47 @@
       <c r="AT27" s="112"/>
     </row>
     <row r="28" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A28" s="186"/>
-      <c r="B28" s="186"/>
-      <c r="C28" s="186"/>
-      <c r="D28" s="186"/>
-      <c r="E28" s="186"/>
-      <c r="F28" s="186"/>
-      <c r="G28" s="186"/>
-      <c r="H28" s="186"/>
-      <c r="I28" s="186"/>
+      <c r="A28" s="184"/>
+      <c r="B28" s="184"/>
+      <c r="C28" s="184"/>
+      <c r="D28" s="184"/>
+      <c r="E28" s="184"/>
+      <c r="F28" s="184"/>
+      <c r="G28" s="184"/>
+      <c r="H28" s="184"/>
+      <c r="I28" s="184"/>
       <c r="AT28" s="112"/>
     </row>
     <row r="29" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="A29" s="186"/>
-      <c r="B29" s="186"/>
-      <c r="C29" s="186"/>
-      <c r="D29" s="186"/>
-      <c r="E29" s="186"/>
-      <c r="F29" s="186"/>
-      <c r="G29" s="186"/>
-      <c r="H29" s="186"/>
-      <c r="I29" s="186"/>
-      <c r="L29" s="186"/>
-      <c r="M29" s="186"/>
-      <c r="N29" s="186"/>
-      <c r="O29" s="186"/>
-      <c r="P29" s="186"/>
-      <c r="Q29" s="186"/>
-      <c r="R29" s="186"/>
-      <c r="S29" s="186"/>
-      <c r="T29" s="186"/>
+      <c r="A29" s="184"/>
+      <c r="B29" s="184"/>
+      <c r="C29" s="184"/>
+      <c r="D29" s="184"/>
+      <c r="E29" s="184"/>
+      <c r="F29" s="184"/>
+      <c r="G29" s="184"/>
+      <c r="H29" s="184"/>
+      <c r="I29" s="184"/>
+      <c r="L29" s="184"/>
+      <c r="M29" s="184"/>
+      <c r="N29" s="184"/>
+      <c r="O29" s="184"/>
+      <c r="P29" s="184"/>
+      <c r="Q29" s="184"/>
+      <c r="R29" s="184"/>
+      <c r="S29" s="184"/>
+      <c r="T29" s="184"/>
     </row>
     <row r="30" spans="1:54" x14ac:dyDescent="0.25">
-      <c r="L30" s="186"/>
-      <c r="M30" s="186"/>
-      <c r="N30" s="186"/>
-      <c r="O30" s="186"/>
-      <c r="P30" s="186"/>
-      <c r="Q30" s="186"/>
-      <c r="R30" s="186"/>
-      <c r="S30" s="186"/>
-      <c r="T30" s="186"/>
+      <c r="L30" s="184"/>
+      <c r="M30" s="184"/>
+      <c r="N30" s="184"/>
+      <c r="O30" s="184"/>
+      <c r="P30" s="184"/>
+      <c r="Q30" s="184"/>
+      <c r="R30" s="184"/>
+      <c r="S30" s="184"/>
+      <c r="T30" s="184"/>
     </row>
     <row r="31" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A31" s="55"/>
@@ -18415,7 +18069,7 @@
         <f>SUM(D32:D36)/(SUM(C32:C36))</f>
         <v>#REF!</v>
       </c>
-      <c r="I31" s="187" t="e">
+      <c r="I31" s="185" t="e">
         <f>GOT!#REF!</f>
         <v>#REF!</v>
       </c>
@@ -18438,7 +18092,7 @@
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20"/>
-      <c r="I32" s="188"/>
+      <c r="I32" s="186"/>
       <c r="L32" s="55"/>
       <c r="M32" s="30" t="s">
         <v>112</v>
@@ -18457,7 +18111,7 @@
         <f>SUM(O33:O37)/(SUM(N33:N37))</f>
         <v>1.9166666666666667</v>
       </c>
-      <c r="T32" s="187">
+      <c r="T32" s="185">
         <f>GOT!C3</f>
         <v>41710</v>
       </c>
@@ -18480,7 +18134,7 @@
       <c r="E33" s="20"/>
       <c r="F33" s="20"/>
       <c r="G33" s="20"/>
-      <c r="I33" s="188"/>
+      <c r="I33" s="186"/>
       <c r="L33" s="58" t="s">
         <v>119</v>
       </c>
@@ -18498,7 +18152,7 @@
       <c r="P33" s="20"/>
       <c r="Q33" s="20"/>
       <c r="R33" s="20"/>
-      <c r="T33" s="188"/>
+      <c r="T33" s="186"/>
     </row>
     <row r="34" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="63" t="s">
@@ -18518,7 +18172,7 @@
       <c r="E34" s="20"/>
       <c r="F34" s="20"/>
       <c r="G34" s="20"/>
-      <c r="I34" s="188"/>
+      <c r="I34" s="186"/>
       <c r="L34" s="61" t="s">
         <v>114</v>
       </c>
@@ -18536,7 +18190,7 @@
       <c r="P34" s="20"/>
       <c r="Q34" s="20"/>
       <c r="R34" s="20"/>
-      <c r="T34" s="188"/>
+      <c r="T34" s="186"/>
     </row>
     <row r="35" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="61" t="s">
@@ -18562,7 +18216,7 @@
         <v>#REF!</v>
       </c>
       <c r="H35" s="20"/>
-      <c r="I35" s="188"/>
+      <c r="I35" s="186"/>
       <c r="L35" s="63" t="s">
         <v>116</v>
       </c>
@@ -18580,7 +18234,7 @@
       <c r="P35" s="20"/>
       <c r="Q35" s="20"/>
       <c r="R35" s="20"/>
-      <c r="T35" s="188"/>
+      <c r="T35" s="186"/>
     </row>
     <row r="36" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="66" t="s">
@@ -18624,7 +18278,7 @@
         <v>2</v>
       </c>
       <c r="S36" s="20"/>
-      <c r="T36" s="188"/>
+      <c r="T36" s="186"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="L37" s="66" t="s">
@@ -18647,46 +18301,46 @@
       <c r="S37" s="20"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="186"/>
-      <c r="B38" s="186"/>
-      <c r="C38" s="186"/>
-      <c r="D38" s="186"/>
-      <c r="E38" s="186"/>
-      <c r="F38" s="186"/>
-      <c r="G38" s="186"/>
-      <c r="H38" s="186"/>
-      <c r="I38" s="186"/>
+      <c r="A38" s="184"/>
+      <c r="B38" s="184"/>
+      <c r="C38" s="184"/>
+      <c r="D38" s="184"/>
+      <c r="E38" s="184"/>
+      <c r="F38" s="184"/>
+      <c r="G38" s="184"/>
+      <c r="H38" s="184"/>
+      <c r="I38" s="184"/>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" s="186"/>
-      <c r="B39" s="186"/>
-      <c r="C39" s="186"/>
-      <c r="D39" s="186"/>
-      <c r="E39" s="186"/>
-      <c r="F39" s="186"/>
-      <c r="G39" s="186"/>
-      <c r="H39" s="186"/>
-      <c r="I39" s="186"/>
-      <c r="L39" s="186"/>
-      <c r="M39" s="186"/>
-      <c r="N39" s="186"/>
-      <c r="O39" s="186"/>
-      <c r="P39" s="186"/>
-      <c r="Q39" s="186"/>
-      <c r="R39" s="186"/>
-      <c r="S39" s="186"/>
-      <c r="T39" s="186"/>
+      <c r="A39" s="184"/>
+      <c r="B39" s="184"/>
+      <c r="C39" s="184"/>
+      <c r="D39" s="184"/>
+      <c r="E39" s="184"/>
+      <c r="F39" s="184"/>
+      <c r="G39" s="184"/>
+      <c r="H39" s="184"/>
+      <c r="I39" s="184"/>
+      <c r="L39" s="184"/>
+      <c r="M39" s="184"/>
+      <c r="N39" s="184"/>
+      <c r="O39" s="184"/>
+      <c r="P39" s="184"/>
+      <c r="Q39" s="184"/>
+      <c r="R39" s="184"/>
+      <c r="S39" s="184"/>
+      <c r="T39" s="184"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="L40" s="186"/>
-      <c r="M40" s="186"/>
-      <c r="N40" s="186"/>
-      <c r="O40" s="186"/>
-      <c r="P40" s="186"/>
-      <c r="Q40" s="186"/>
-      <c r="R40" s="186"/>
-      <c r="S40" s="186"/>
-      <c r="T40" s="186"/>
+      <c r="L40" s="184"/>
+      <c r="M40" s="184"/>
+      <c r="N40" s="184"/>
+      <c r="O40" s="184"/>
+      <c r="P40" s="184"/>
+      <c r="Q40" s="184"/>
+      <c r="R40" s="184"/>
+      <c r="S40" s="184"/>
+      <c r="T40" s="184"/>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="55"/>
@@ -18707,7 +18361,7 @@
         <f>SUM(D42:D46)/(SUM(C42:C46))</f>
         <v>#REF!</v>
       </c>
-      <c r="I41" s="187" t="e">
+      <c r="I41" s="185" t="e">
         <f>GOT!#REF!</f>
         <v>#REF!</v>
       </c>
@@ -18730,7 +18384,7 @@
       <c r="E42" s="20"/>
       <c r="F42" s="20"/>
       <c r="G42" s="20"/>
-      <c r="I42" s="188"/>
+      <c r="I42" s="186"/>
       <c r="L42" s="55"/>
       <c r="M42" s="30" t="s">
         <v>112</v>
@@ -18749,7 +18403,7 @@
         <f>SUM(O43:O47)/(SUM(N43:N47))</f>
         <v>1.9166666666666667</v>
       </c>
-      <c r="T42" s="187">
+      <c r="T42" s="185">
         <f>GOT!B3</f>
         <v>42333.395833333336</v>
       </c>
@@ -18772,7 +18426,7 @@
       <c r="E43" s="20"/>
       <c r="F43" s="20"/>
       <c r="G43" s="20"/>
-      <c r="I43" s="188"/>
+      <c r="I43" s="186"/>
       <c r="L43" s="58" t="s">
         <v>119</v>
       </c>
@@ -18790,7 +18444,7 @@
       <c r="P43" s="20"/>
       <c r="Q43" s="20"/>
       <c r="R43" s="20"/>
-      <c r="T43" s="188"/>
+      <c r="T43" s="186"/>
     </row>
     <row r="44" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="63" t="s">
@@ -18810,7 +18464,7 @@
       <c r="E44" s="20"/>
       <c r="F44" s="20"/>
       <c r="G44" s="20"/>
-      <c r="I44" s="188"/>
+      <c r="I44" s="186"/>
       <c r="L44" s="61" t="s">
         <v>114</v>
       </c>
@@ -18828,7 +18482,7 @@
       <c r="P44" s="20"/>
       <c r="Q44" s="20"/>
       <c r="R44" s="20"/>
-      <c r="T44" s="188"/>
+      <c r="T44" s="186"/>
     </row>
     <row r="45" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="61" t="s">
@@ -18854,7 +18508,7 @@
         <v>#REF!</v>
       </c>
       <c r="H45" s="20"/>
-      <c r="I45" s="188"/>
+      <c r="I45" s="186"/>
       <c r="L45" s="63" t="s">
         <v>116</v>
       </c>
@@ -18872,7 +18526,7 @@
       <c r="P45" s="20"/>
       <c r="Q45" s="20"/>
       <c r="R45" s="20"/>
-      <c r="T45" s="188"/>
+      <c r="T45" s="186"/>
     </row>
     <row r="46" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="66" t="s">
@@ -18916,7 +18570,7 @@
         <v>2</v>
       </c>
       <c r="S46" s="20"/>
-      <c r="T46" s="188"/>
+      <c r="T46" s="186"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="L47" s="66" t="s">
@@ -18939,26 +18593,26 @@
       <c r="S47" s="20"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A48" s="186"/>
-      <c r="B48" s="186"/>
-      <c r="C48" s="186"/>
-      <c r="D48" s="186"/>
-      <c r="E48" s="186"/>
-      <c r="F48" s="186"/>
-      <c r="G48" s="186"/>
-      <c r="H48" s="186"/>
-      <c r="I48" s="186"/>
+      <c r="A48" s="184"/>
+      <c r="B48" s="184"/>
+      <c r="C48" s="184"/>
+      <c r="D48" s="184"/>
+      <c r="E48" s="184"/>
+      <c r="F48" s="184"/>
+      <c r="G48" s="184"/>
+      <c r="H48" s="184"/>
+      <c r="I48" s="184"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A49" s="186"/>
-      <c r="B49" s="186"/>
-      <c r="C49" s="186"/>
-      <c r="D49" s="186"/>
-      <c r="E49" s="186"/>
-      <c r="F49" s="186"/>
-      <c r="G49" s="186"/>
-      <c r="H49" s="186"/>
-      <c r="I49" s="186"/>
+      <c r="A49" s="184"/>
+      <c r="B49" s="184"/>
+      <c r="C49" s="184"/>
+      <c r="D49" s="184"/>
+      <c r="E49" s="184"/>
+      <c r="F49" s="184"/>
+      <c r="G49" s="184"/>
+      <c r="H49" s="184"/>
+      <c r="I49" s="184"/>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="55"/>
@@ -18979,7 +18633,7 @@
         <f>SUM(D52:D56)/(SUM(C52:C56))</f>
         <v>#REF!</v>
       </c>
-      <c r="I51" s="187" t="e">
+      <c r="I51" s="185" t="e">
         <f>GOT!#REF!</f>
         <v>#REF!</v>
       </c>
@@ -19002,7 +18656,7 @@
       <c r="E52" s="20"/>
       <c r="F52" s="20"/>
       <c r="G52" s="20"/>
-      <c r="I52" s="188"/>
+      <c r="I52" s="186"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="61" t="s">
@@ -19022,7 +18676,7 @@
       <c r="E53" s="20"/>
       <c r="F53" s="20"/>
       <c r="G53" s="20"/>
-      <c r="I53" s="188"/>
+      <c r="I53" s="186"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="63" t="s">
@@ -19042,7 +18696,7 @@
       <c r="E54" s="20"/>
       <c r="F54" s="20"/>
       <c r="G54" s="20"/>
-      <c r="I54" s="188"/>
+      <c r="I54" s="186"/>
       <c r="N54" s="125"/>
       <c r="O54" s="125"/>
       <c r="P54" s="133"/>
@@ -19072,7 +18726,7 @@
         <v>#REF!</v>
       </c>
       <c r="H55" s="20"/>
-      <c r="I55" s="188"/>
+      <c r="I55" s="186"/>
       <c r="N55" s="15"/>
       <c r="O55" s="126"/>
       <c r="P55" s="133"/>
@@ -19109,30 +18763,30 @@
       <c r="Q57" s="131"/>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A58" s="186"/>
-      <c r="B58" s="186"/>
-      <c r="C58" s="186"/>
-      <c r="D58" s="186"/>
-      <c r="E58" s="186"/>
-      <c r="F58" s="186"/>
-      <c r="G58" s="186"/>
-      <c r="H58" s="186"/>
-      <c r="I58" s="186"/>
+      <c r="A58" s="184"/>
+      <c r="B58" s="184"/>
+      <c r="C58" s="184"/>
+      <c r="D58" s="184"/>
+      <c r="E58" s="184"/>
+      <c r="F58" s="184"/>
+      <c r="G58" s="184"/>
+      <c r="H58" s="184"/>
+      <c r="I58" s="184"/>
       <c r="N58" s="130"/>
       <c r="O58" s="116"/>
       <c r="P58" s="116"/>
       <c r="Q58" s="131"/>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A59" s="186"/>
-      <c r="B59" s="186"/>
-      <c r="C59" s="186"/>
-      <c r="D59" s="186"/>
-      <c r="E59" s="186"/>
-      <c r="F59" s="186"/>
-      <c r="G59" s="186"/>
-      <c r="H59" s="186"/>
-      <c r="I59" s="186"/>
+      <c r="A59" s="184"/>
+      <c r="B59" s="184"/>
+      <c r="C59" s="184"/>
+      <c r="D59" s="184"/>
+      <c r="E59" s="184"/>
+      <c r="F59" s="184"/>
+      <c r="G59" s="184"/>
+      <c r="H59" s="184"/>
+      <c r="I59" s="184"/>
       <c r="N59" s="130"/>
       <c r="O59" s="116"/>
       <c r="P59" s="116"/>
@@ -19163,7 +18817,7 @@
         <f>SUM(D62:D66)/(SUM(C62:C66))</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="I61" s="187">
+      <c r="I61" s="185">
         <f>GOT!R3</f>
         <v>34374</v>
       </c>
@@ -19190,7 +18844,7 @@
       <c r="E62" s="20"/>
       <c r="F62" s="20"/>
       <c r="G62" s="20"/>
-      <c r="I62" s="188"/>
+      <c r="I62" s="186"/>
       <c r="N62" s="132"/>
       <c r="O62" s="116"/>
       <c r="P62" s="116"/>
@@ -19214,7 +18868,7 @@
       <c r="E63" s="20"/>
       <c r="F63" s="20"/>
       <c r="G63" s="20"/>
-      <c r="I63" s="188"/>
+      <c r="I63" s="186"/>
       <c r="N63" s="132"/>
       <c r="O63" s="127"/>
       <c r="P63" s="116"/>
@@ -19238,7 +18892,7 @@
       <c r="E64" s="20"/>
       <c r="F64" s="20"/>
       <c r="G64" s="20"/>
-      <c r="I64" s="188"/>
+      <c r="I64" s="186"/>
       <c r="N64" s="129"/>
       <c r="O64" s="116"/>
       <c r="P64" s="116"/>
@@ -19268,7 +18922,7 @@
         <v>4</v>
       </c>
       <c r="H65" s="20"/>
-      <c r="I65" s="188"/>
+      <c r="I65" s="186"/>
       <c r="N65" s="130"/>
       <c r="O65" s="116"/>
       <c r="P65" s="116"/>
@@ -19305,15 +18959,15 @@
       <c r="Q67" s="131"/>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A68" s="186"/>
-      <c r="B68" s="186"/>
-      <c r="C68" s="186"/>
-      <c r="D68" s="186"/>
-      <c r="E68" s="186"/>
-      <c r="F68" s="186"/>
-      <c r="G68" s="186"/>
-      <c r="H68" s="186"/>
-      <c r="I68" s="186"/>
+      <c r="A68" s="184"/>
+      <c r="B68" s="184"/>
+      <c r="C68" s="184"/>
+      <c r="D68" s="184"/>
+      <c r="E68" s="184"/>
+      <c r="F68" s="184"/>
+      <c r="G68" s="184"/>
+      <c r="H68" s="184"/>
+      <c r="I68" s="184"/>
       <c r="J68" s="20"/>
       <c r="N68" s="132"/>
       <c r="O68" s="116"/>
@@ -19321,15 +18975,15 @@
       <c r="Q68" s="131"/>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A69" s="186"/>
-      <c r="B69" s="186"/>
-      <c r="C69" s="186"/>
-      <c r="D69" s="186"/>
-      <c r="E69" s="186"/>
-      <c r="F69" s="186"/>
-      <c r="G69" s="186"/>
-      <c r="H69" s="186"/>
-      <c r="I69" s="186"/>
+      <c r="A69" s="184"/>
+      <c r="B69" s="184"/>
+      <c r="C69" s="184"/>
+      <c r="D69" s="184"/>
+      <c r="E69" s="184"/>
+      <c r="F69" s="184"/>
+      <c r="G69" s="184"/>
+      <c r="H69" s="184"/>
+      <c r="I69" s="184"/>
       <c r="J69" s="20"/>
       <c r="N69" s="132"/>
       <c r="O69" s="116"/>
@@ -19362,7 +19016,7 @@
         <f>SUM(D72:D76)/(SUM(C72:C76))</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="I71" s="187">
+      <c r="I71" s="185">
         <f>GOT!Q3</f>
         <v>35460</v>
       </c>
@@ -19390,7 +19044,7 @@
       <c r="E72" s="20"/>
       <c r="F72" s="20"/>
       <c r="G72" s="20"/>
-      <c r="I72" s="188"/>
+      <c r="I72" s="186"/>
       <c r="J72" s="20"/>
       <c r="N72" s="129"/>
       <c r="O72" s="127"/>
@@ -19415,7 +19069,7 @@
       <c r="E73" s="20"/>
       <c r="F73" s="20"/>
       <c r="G73" s="20"/>
-      <c r="I73" s="188"/>
+      <c r="I73" s="186"/>
       <c r="J73" s="20"/>
       <c r="N73" s="130"/>
       <c r="O73" s="128"/>
@@ -19440,7 +19094,7 @@
       <c r="E74" s="20"/>
       <c r="F74" s="20"/>
       <c r="G74" s="20"/>
-      <c r="I74" s="188"/>
+      <c r="I74" s="186"/>
       <c r="J74" s="20"/>
       <c r="N74" s="130"/>
       <c r="O74" s="128"/>
@@ -19471,7 +19125,7 @@
         <v>4</v>
       </c>
       <c r="H75" s="20"/>
-      <c r="I75" s="188"/>
+      <c r="I75" s="186"/>
       <c r="J75" s="20"/>
       <c r="N75" s="130"/>
       <c r="O75" s="128"/>
@@ -19503,27 +19157,27 @@
       <c r="J77" s="36"/>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A78" s="186"/>
-      <c r="B78" s="186"/>
-      <c r="C78" s="186"/>
-      <c r="D78" s="186"/>
-      <c r="E78" s="186"/>
-      <c r="F78" s="186"/>
-      <c r="G78" s="186"/>
-      <c r="H78" s="186"/>
-      <c r="I78" s="186"/>
+      <c r="A78" s="184"/>
+      <c r="B78" s="184"/>
+      <c r="C78" s="184"/>
+      <c r="D78" s="184"/>
+      <c r="E78" s="184"/>
+      <c r="F78" s="184"/>
+      <c r="G78" s="184"/>
+      <c r="H78" s="184"/>
+      <c r="I78" s="184"/>
       <c r="J78" s="36"/>
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A79" s="186"/>
-      <c r="B79" s="186"/>
-      <c r="C79" s="186"/>
-      <c r="D79" s="186"/>
-      <c r="E79" s="186"/>
-      <c r="F79" s="186"/>
-      <c r="G79" s="186"/>
-      <c r="H79" s="186"/>
-      <c r="I79" s="186"/>
+      <c r="A79" s="184"/>
+      <c r="B79" s="184"/>
+      <c r="C79" s="184"/>
+      <c r="D79" s="184"/>
+      <c r="E79" s="184"/>
+      <c r="F79" s="184"/>
+      <c r="G79" s="184"/>
+      <c r="H79" s="184"/>
+      <c r="I79" s="184"/>
       <c r="J79" s="36"/>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
@@ -19548,7 +19202,7 @@
         <f>SUM(D82:D86)/(SUM(C82:C86))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="I81" s="187">
+      <c r="I81" s="185">
         <f>GOT!P3</f>
         <v>35827</v>
       </c>
@@ -19572,7 +19226,7 @@
       <c r="E82" s="20"/>
       <c r="F82" s="20"/>
       <c r="G82" s="20"/>
-      <c r="I82" s="188"/>
+      <c r="I82" s="186"/>
       <c r="J82" s="36"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
@@ -19593,7 +19247,7 @@
       <c r="E83" s="20"/>
       <c r="F83" s="20"/>
       <c r="G83" s="20"/>
-      <c r="I83" s="188"/>
+      <c r="I83" s="186"/>
       <c r="J83" s="36"/>
     </row>
     <row r="84" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -19614,7 +19268,7 @@
       <c r="E84" s="20"/>
       <c r="F84" s="20"/>
       <c r="G84" s="20"/>
-      <c r="I84" s="188"/>
+      <c r="I84" s="186"/>
     </row>
     <row r="85" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="61" t="s">
@@ -19640,7 +19294,7 @@
         <v>3</v>
       </c>
       <c r="H85" s="20"/>
-      <c r="I85" s="188"/>
+      <c r="I85" s="186"/>
       <c r="J85" s="20"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
@@ -19668,27 +19322,27 @@
       <c r="J87" s="20"/>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="186"/>
-      <c r="B88" s="186"/>
-      <c r="C88" s="186"/>
-      <c r="D88" s="186"/>
-      <c r="E88" s="186"/>
-      <c r="F88" s="186"/>
-      <c r="G88" s="186"/>
-      <c r="H88" s="186"/>
-      <c r="I88" s="186"/>
+      <c r="A88" s="184"/>
+      <c r="B88" s="184"/>
+      <c r="C88" s="184"/>
+      <c r="D88" s="184"/>
+      <c r="E88" s="184"/>
+      <c r="F88" s="184"/>
+      <c r="G88" s="184"/>
+      <c r="H88" s="184"/>
+      <c r="I88" s="184"/>
       <c r="J88" s="20"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="186"/>
-      <c r="B89" s="186"/>
-      <c r="C89" s="186"/>
-      <c r="D89" s="186"/>
-      <c r="E89" s="186"/>
-      <c r="F89" s="186"/>
-      <c r="G89" s="186"/>
-      <c r="H89" s="186"/>
-      <c r="I89" s="186"/>
+      <c r="A89" s="184"/>
+      <c r="B89" s="184"/>
+      <c r="C89" s="184"/>
+      <c r="D89" s="184"/>
+      <c r="E89" s="184"/>
+      <c r="F89" s="184"/>
+      <c r="G89" s="184"/>
+      <c r="H89" s="184"/>
+      <c r="I89" s="184"/>
       <c r="J89" s="20"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
@@ -19713,7 +19367,7 @@
         <f>SUM(D92:D96)/(SUM(C92:C96))</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="I91" s="187">
+      <c r="I91" s="185">
         <f>GOT!O3</f>
         <v>36166</v>
       </c>
@@ -19737,7 +19391,7 @@
       <c r="E92" s="20"/>
       <c r="F92" s="20"/>
       <c r="G92" s="20"/>
-      <c r="I92" s="188"/>
+      <c r="I92" s="186"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="61" t="s">
@@ -19757,7 +19411,7 @@
       <c r="E93" s="20"/>
       <c r="F93" s="20"/>
       <c r="G93" s="20"/>
-      <c r="I93" s="188"/>
+      <c r="I93" s="186"/>
     </row>
     <row r="94" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="63" t="s">
@@ -19777,7 +19431,7 @@
       <c r="E94" s="20"/>
       <c r="F94" s="20"/>
       <c r="G94" s="20"/>
-      <c r="I94" s="188"/>
+      <c r="I94" s="186"/>
     </row>
     <row r="95" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="61" t="s">
@@ -19803,7 +19457,7 @@
         <v>4</v>
       </c>
       <c r="H95" s="20"/>
-      <c r="I95" s="188"/>
+      <c r="I95" s="186"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="66" t="s">
@@ -19826,26 +19480,26 @@
       <c r="H96" s="20"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="186"/>
-      <c r="B98" s="186"/>
-      <c r="C98" s="186"/>
-      <c r="D98" s="186"/>
-      <c r="E98" s="186"/>
-      <c r="F98" s="186"/>
-      <c r="G98" s="186"/>
-      <c r="H98" s="186"/>
-      <c r="I98" s="186"/>
+      <c r="A98" s="184"/>
+      <c r="B98" s="184"/>
+      <c r="C98" s="184"/>
+      <c r="D98" s="184"/>
+      <c r="E98" s="184"/>
+      <c r="F98" s="184"/>
+      <c r="G98" s="184"/>
+      <c r="H98" s="184"/>
+      <c r="I98" s="184"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="186"/>
-      <c r="B99" s="186"/>
-      <c r="C99" s="186"/>
-      <c r="D99" s="186"/>
-      <c r="E99" s="186"/>
-      <c r="F99" s="186"/>
-      <c r="G99" s="186"/>
-      <c r="H99" s="186"/>
-      <c r="I99" s="186"/>
+      <c r="A99" s="184"/>
+      <c r="B99" s="184"/>
+      <c r="C99" s="184"/>
+      <c r="D99" s="184"/>
+      <c r="E99" s="184"/>
+      <c r="F99" s="184"/>
+      <c r="G99" s="184"/>
+      <c r="H99" s="184"/>
+      <c r="I99" s="184"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="55"/>
@@ -19866,7 +19520,7 @@
         <f>SUM(D102:D106)/(SUM(C102:C106))</f>
         <v>1.1666666666666667</v>
       </c>
-      <c r="I101" s="187">
+      <c r="I101" s="185">
         <f>GOT!N3</f>
         <v>36684</v>
       </c>
@@ -19889,7 +19543,7 @@
       <c r="E102" s="20"/>
       <c r="F102" s="20"/>
       <c r="G102" s="20"/>
-      <c r="I102" s="188"/>
+      <c r="I102" s="186"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="61" t="s">
@@ -19909,7 +19563,7 @@
       <c r="E103" s="20"/>
       <c r="F103" s="20"/>
       <c r="G103" s="20"/>
-      <c r="I103" s="188"/>
+      <c r="I103" s="186"/>
     </row>
     <row r="104" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="63" t="s">
@@ -19929,7 +19583,7 @@
       <c r="E104" s="20"/>
       <c r="F104" s="20"/>
       <c r="G104" s="20"/>
-      <c r="I104" s="188"/>
+      <c r="I104" s="186"/>
     </row>
     <row r="105" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="61" t="s">
@@ -19955,7 +19609,7 @@
         <v>4</v>
       </c>
       <c r="H105" s="20"/>
-      <c r="I105" s="188"/>
+      <c r="I105" s="186"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="66" t="s">
@@ -19978,26 +19632,26 @@
       <c r="H106" s="20"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="186"/>
-      <c r="B108" s="186"/>
-      <c r="C108" s="186"/>
-      <c r="D108" s="186"/>
-      <c r="E108" s="186"/>
-      <c r="F108" s="186"/>
-      <c r="G108" s="186"/>
-      <c r="H108" s="186"/>
-      <c r="I108" s="186"/>
+      <c r="A108" s="184"/>
+      <c r="B108" s="184"/>
+      <c r="C108" s="184"/>
+      <c r="D108" s="184"/>
+      <c r="E108" s="184"/>
+      <c r="F108" s="184"/>
+      <c r="G108" s="184"/>
+      <c r="H108" s="184"/>
+      <c r="I108" s="184"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="186"/>
-      <c r="B109" s="186"/>
-      <c r="C109" s="186"/>
-      <c r="D109" s="186"/>
-      <c r="E109" s="186"/>
-      <c r="F109" s="186"/>
-      <c r="G109" s="186"/>
-      <c r="H109" s="186"/>
-      <c r="I109" s="186"/>
+      <c r="A109" s="184"/>
+      <c r="B109" s="184"/>
+      <c r="C109" s="184"/>
+      <c r="D109" s="184"/>
+      <c r="E109" s="184"/>
+      <c r="F109" s="184"/>
+      <c r="G109" s="184"/>
+      <c r="H109" s="184"/>
+      <c r="I109" s="184"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="55"/>
@@ -20018,7 +19672,7 @@
         <f>SUM(D112:D116)/(SUM(C112:C116))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="I111" s="187">
+      <c r="I111" s="185">
         <f>GOT!M3</f>
         <v>37062</v>
       </c>
@@ -20041,7 +19695,7 @@
       <c r="E112" s="20"/>
       <c r="F112" s="20"/>
       <c r="G112" s="20"/>
-      <c r="I112" s="188"/>
+      <c r="I112" s="186"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="61" t="s">
@@ -20061,7 +19715,7 @@
       <c r="E113" s="20"/>
       <c r="F113" s="20"/>
       <c r="G113" s="20"/>
-      <c r="I113" s="188"/>
+      <c r="I113" s="186"/>
     </row>
     <row r="114" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="63" t="s">
@@ -20081,7 +19735,7 @@
       <c r="E114" s="20"/>
       <c r="F114" s="20"/>
       <c r="G114" s="20"/>
-      <c r="I114" s="188"/>
+      <c r="I114" s="186"/>
     </row>
     <row r="115" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="61" t="s">
@@ -20107,7 +19761,7 @@
         <v>3</v>
       </c>
       <c r="H115" s="20"/>
-      <c r="I115" s="188"/>
+      <c r="I115" s="186"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="66" t="s">
@@ -20130,26 +19784,26 @@
       <c r="H116" s="20"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118" s="186"/>
-      <c r="B118" s="186"/>
-      <c r="C118" s="186"/>
-      <c r="D118" s="186"/>
-      <c r="E118" s="186"/>
-      <c r="F118" s="186"/>
-      <c r="G118" s="186"/>
-      <c r="H118" s="186"/>
-      <c r="I118" s="186"/>
+      <c r="A118" s="184"/>
+      <c r="B118" s="184"/>
+      <c r="C118" s="184"/>
+      <c r="D118" s="184"/>
+      <c r="E118" s="184"/>
+      <c r="F118" s="184"/>
+      <c r="G118" s="184"/>
+      <c r="H118" s="184"/>
+      <c r="I118" s="184"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="186"/>
-      <c r="B119" s="186"/>
-      <c r="C119" s="186"/>
-      <c r="D119" s="186"/>
-      <c r="E119" s="186"/>
-      <c r="F119" s="186"/>
-      <c r="G119" s="186"/>
-      <c r="H119" s="186"/>
-      <c r="I119" s="186"/>
+      <c r="A119" s="184"/>
+      <c r="B119" s="184"/>
+      <c r="C119" s="184"/>
+      <c r="D119" s="184"/>
+      <c r="E119" s="184"/>
+      <c r="F119" s="184"/>
+      <c r="G119" s="184"/>
+      <c r="H119" s="184"/>
+      <c r="I119" s="184"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="55"/>
@@ -20170,7 +19824,7 @@
         <f>SUM(D122:D126)/(SUM(C122:C126))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="I121" s="187">
+      <c r="I121" s="185">
         <f>GOT!L3</f>
         <v>37321</v>
       </c>
@@ -20193,7 +19847,7 @@
       <c r="E122" s="20"/>
       <c r="F122" s="20"/>
       <c r="G122" s="20"/>
-      <c r="I122" s="188"/>
+      <c r="I122" s="186"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="61" t="s">
@@ -20213,7 +19867,7 @@
       <c r="E123" s="20"/>
       <c r="F123" s="20"/>
       <c r="G123" s="20"/>
-      <c r="I123" s="188"/>
+      <c r="I123" s="186"/>
     </row>
     <row r="124" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="63" t="s">
@@ -20233,7 +19887,7 @@
       <c r="E124" s="20"/>
       <c r="F124" s="20"/>
       <c r="G124" s="20"/>
-      <c r="I124" s="188"/>
+      <c r="I124" s="186"/>
     </row>
     <row r="125" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="61" t="s">
@@ -20259,7 +19913,7 @@
         <v>3</v>
       </c>
       <c r="H125" s="20"/>
-      <c r="I125" s="188"/>
+      <c r="I125" s="186"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="66" t="s">
@@ -20282,26 +19936,26 @@
       <c r="H126" s="20"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A128" s="186"/>
-      <c r="B128" s="186"/>
-      <c r="C128" s="186"/>
-      <c r="D128" s="186"/>
-      <c r="E128" s="186"/>
-      <c r="F128" s="186"/>
-      <c r="G128" s="186"/>
-      <c r="H128" s="186"/>
-      <c r="I128" s="186"/>
+      <c r="A128" s="184"/>
+      <c r="B128" s="184"/>
+      <c r="C128" s="184"/>
+      <c r="D128" s="184"/>
+      <c r="E128" s="184"/>
+      <c r="F128" s="184"/>
+      <c r="G128" s="184"/>
+      <c r="H128" s="184"/>
+      <c r="I128" s="184"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A129" s="186"/>
-      <c r="B129" s="186"/>
-      <c r="C129" s="186"/>
-      <c r="D129" s="186"/>
-      <c r="E129" s="186"/>
-      <c r="F129" s="186"/>
-      <c r="G129" s="186"/>
-      <c r="H129" s="186"/>
-      <c r="I129" s="186"/>
+      <c r="A129" s="184"/>
+      <c r="B129" s="184"/>
+      <c r="C129" s="184"/>
+      <c r="D129" s="184"/>
+      <c r="E129" s="184"/>
+      <c r="F129" s="184"/>
+      <c r="G129" s="184"/>
+      <c r="H129" s="184"/>
+      <c r="I129" s="184"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="55"/>
@@ -20322,7 +19976,7 @@
         <f>SUM(D132:D136)/(SUM(C132:C136))</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="I131" s="187">
+      <c r="I131" s="185">
         <f>GOT!K3</f>
         <v>37649</v>
       </c>
@@ -20345,7 +19999,7 @@
       <c r="E132" s="20"/>
       <c r="F132" s="20"/>
       <c r="G132" s="20"/>
-      <c r="I132" s="188"/>
+      <c r="I132" s="186"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="61" t="s">
@@ -20365,7 +20019,7 @@
       <c r="E133" s="20"/>
       <c r="F133" s="20"/>
       <c r="G133" s="20"/>
-      <c r="I133" s="188"/>
+      <c r="I133" s="186"/>
     </row>
     <row r="134" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="63" t="s">
@@ -20385,7 +20039,7 @@
       <c r="E134" s="20"/>
       <c r="F134" s="20"/>
       <c r="G134" s="20"/>
-      <c r="I134" s="188"/>
+      <c r="I134" s="186"/>
     </row>
     <row r="135" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="61" t="s">
@@ -20411,7 +20065,7 @@
         <v>3</v>
       </c>
       <c r="H135" s="20"/>
-      <c r="I135" s="188"/>
+      <c r="I135" s="186"/>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="66" t="s">
@@ -20444,26 +20098,26 @@
       <c r="H137" s="20"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A138" s="186"/>
-      <c r="B138" s="186"/>
-      <c r="C138" s="186"/>
-      <c r="D138" s="186"/>
-      <c r="E138" s="186"/>
-      <c r="F138" s="186"/>
-      <c r="G138" s="186"/>
-      <c r="H138" s="186"/>
-      <c r="I138" s="186"/>
+      <c r="A138" s="184"/>
+      <c r="B138" s="184"/>
+      <c r="C138" s="184"/>
+      <c r="D138" s="184"/>
+      <c r="E138" s="184"/>
+      <c r="F138" s="184"/>
+      <c r="G138" s="184"/>
+      <c r="H138" s="184"/>
+      <c r="I138" s="184"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A139" s="186"/>
-      <c r="B139" s="186"/>
-      <c r="C139" s="186"/>
-      <c r="D139" s="186"/>
-      <c r="E139" s="186"/>
-      <c r="F139" s="186"/>
-      <c r="G139" s="186"/>
-      <c r="H139" s="186"/>
-      <c r="I139" s="186"/>
+      <c r="A139" s="184"/>
+      <c r="B139" s="184"/>
+      <c r="C139" s="184"/>
+      <c r="D139" s="184"/>
+      <c r="E139" s="184"/>
+      <c r="F139" s="184"/>
+      <c r="G139" s="184"/>
+      <c r="H139" s="184"/>
+      <c r="I139" s="184"/>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="55"/>
@@ -20484,7 +20138,7 @@
         <f>SUM(D142:D146)/(SUM(C142:C146))</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="I141" s="187">
+      <c r="I141" s="185">
         <f>GOT!J3</f>
         <v>38015</v>
       </c>
@@ -20507,7 +20161,7 @@
       <c r="E142" s="20"/>
       <c r="F142" s="20"/>
       <c r="G142" s="20"/>
-      <c r="I142" s="188"/>
+      <c r="I142" s="186"/>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="61" t="s">
@@ -20527,7 +20181,7 @@
       <c r="E143" s="20"/>
       <c r="F143" s="20"/>
       <c r="G143" s="20"/>
-      <c r="I143" s="188"/>
+      <c r="I143" s="186"/>
     </row>
     <row r="144" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="63" t="s">
@@ -20547,7 +20201,7 @@
       <c r="E144" s="20"/>
       <c r="F144" s="20"/>
       <c r="G144" s="20"/>
-      <c r="I144" s="188"/>
+      <c r="I144" s="186"/>
     </row>
     <row r="145" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A145" s="61" t="s">
@@ -20573,7 +20227,7 @@
         <v>2</v>
       </c>
       <c r="H145" s="20"/>
-      <c r="I145" s="188"/>
+      <c r="I145" s="186"/>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="66" t="s">
@@ -20596,26 +20250,26 @@
       <c r="H146" s="20"/>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A148" s="186"/>
-      <c r="B148" s="186"/>
-      <c r="C148" s="186"/>
-      <c r="D148" s="186"/>
-      <c r="E148" s="186"/>
-      <c r="F148" s="186"/>
-      <c r="G148" s="186"/>
-      <c r="H148" s="186"/>
-      <c r="I148" s="186"/>
+      <c r="A148" s="184"/>
+      <c r="B148" s="184"/>
+      <c r="C148" s="184"/>
+      <c r="D148" s="184"/>
+      <c r="E148" s="184"/>
+      <c r="F148" s="184"/>
+      <c r="G148" s="184"/>
+      <c r="H148" s="184"/>
+      <c r="I148" s="184"/>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A149" s="186"/>
-      <c r="B149" s="186"/>
-      <c r="C149" s="186"/>
-      <c r="D149" s="186"/>
-      <c r="E149" s="186"/>
-      <c r="F149" s="186"/>
-      <c r="G149" s="186"/>
-      <c r="H149" s="186"/>
-      <c r="I149" s="186"/>
+      <c r="A149" s="184"/>
+      <c r="B149" s="184"/>
+      <c r="C149" s="184"/>
+      <c r="D149" s="184"/>
+      <c r="E149" s="184"/>
+      <c r="F149" s="184"/>
+      <c r="G149" s="184"/>
+      <c r="H149" s="184"/>
+      <c r="I149" s="184"/>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="55"/>
@@ -20636,7 +20290,7 @@
         <f>SUM(D152:D156)/(SUM(C152:C156))</f>
         <v>1.75</v>
       </c>
-      <c r="I151" s="187">
+      <c r="I151" s="185">
         <f>GOT!I3</f>
         <v>38414</v>
       </c>
@@ -20659,7 +20313,7 @@
       <c r="E152" s="20"/>
       <c r="F152" s="20"/>
       <c r="G152" s="20"/>
-      <c r="I152" s="188"/>
+      <c r="I152" s="186"/>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="61" t="s">
@@ -20679,7 +20333,7 @@
       <c r="E153" s="20"/>
       <c r="F153" s="20"/>
       <c r="G153" s="20"/>
-      <c r="I153" s="188"/>
+      <c r="I153" s="186"/>
     </row>
     <row r="154" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="63" t="s">
@@ -20699,7 +20353,7 @@
       <c r="E154" s="20"/>
       <c r="F154" s="20"/>
       <c r="G154" s="20"/>
-      <c r="I154" s="188"/>
+      <c r="I154" s="186"/>
     </row>
     <row r="155" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="61" t="s">
@@ -20725,7 +20379,7 @@
         <v>2</v>
       </c>
       <c r="H155" s="20"/>
-      <c r="I155" s="188"/>
+      <c r="I155" s="186"/>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="66" t="s">
@@ -20748,26 +20402,26 @@
       <c r="H156" s="20"/>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A158" s="186"/>
-      <c r="B158" s="186"/>
-      <c r="C158" s="186"/>
-      <c r="D158" s="186"/>
-      <c r="E158" s="186"/>
-      <c r="F158" s="186"/>
-      <c r="G158" s="186"/>
-      <c r="H158" s="186"/>
-      <c r="I158" s="186"/>
+      <c r="A158" s="184"/>
+      <c r="B158" s="184"/>
+      <c r="C158" s="184"/>
+      <c r="D158" s="184"/>
+      <c r="E158" s="184"/>
+      <c r="F158" s="184"/>
+      <c r="G158" s="184"/>
+      <c r="H158" s="184"/>
+      <c r="I158" s="184"/>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A159" s="186"/>
-      <c r="B159" s="186"/>
-      <c r="C159" s="186"/>
-      <c r="D159" s="186"/>
-      <c r="E159" s="186"/>
-      <c r="F159" s="186"/>
-      <c r="G159" s="186"/>
-      <c r="H159" s="186"/>
-      <c r="I159" s="186"/>
+      <c r="A159" s="184"/>
+      <c r="B159" s="184"/>
+      <c r="C159" s="184"/>
+      <c r="D159" s="184"/>
+      <c r="E159" s="184"/>
+      <c r="F159" s="184"/>
+      <c r="G159" s="184"/>
+      <c r="H159" s="184"/>
+      <c r="I159" s="184"/>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="55"/>
@@ -20788,7 +20442,7 @@
         <f>SUM(D162:D166)/(SUM(C162:C166))</f>
         <v>1.75</v>
       </c>
-      <c r="I161" s="187">
+      <c r="I161" s="185">
         <f>GOT!H3</f>
         <v>38777</v>
       </c>
@@ -20811,7 +20465,7 @@
       <c r="E162" s="20"/>
       <c r="F162" s="20"/>
       <c r="G162" s="20"/>
-      <c r="I162" s="188"/>
+      <c r="I162" s="186"/>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="61" t="s">
@@ -20831,7 +20485,7 @@
       <c r="E163" s="20"/>
       <c r="F163" s="20"/>
       <c r="G163" s="20"/>
-      <c r="I163" s="188"/>
+      <c r="I163" s="186"/>
     </row>
     <row r="164" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="63" t="s">
@@ -20851,7 +20505,7 @@
       <c r="E164" s="20"/>
       <c r="F164" s="20"/>
       <c r="G164" s="20"/>
-      <c r="I164" s="188"/>
+      <c r="I164" s="186"/>
     </row>
     <row r="165" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="61" t="s">
@@ -20877,7 +20531,7 @@
         <v>2</v>
       </c>
       <c r="H165" s="20"/>
-      <c r="I165" s="188"/>
+      <c r="I165" s="186"/>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="66" t="s">
@@ -20900,26 +20554,26 @@
       <c r="H166" s="20"/>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A168" s="186"/>
-      <c r="B168" s="186"/>
-      <c r="C168" s="186"/>
-      <c r="D168" s="186"/>
-      <c r="E168" s="186"/>
-      <c r="F168" s="186"/>
-      <c r="G168" s="186"/>
-      <c r="H168" s="186"/>
-      <c r="I168" s="186"/>
+      <c r="A168" s="184"/>
+      <c r="B168" s="184"/>
+      <c r="C168" s="184"/>
+      <c r="D168" s="184"/>
+      <c r="E168" s="184"/>
+      <c r="F168" s="184"/>
+      <c r="G168" s="184"/>
+      <c r="H168" s="184"/>
+      <c r="I168" s="184"/>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A169" s="186"/>
-      <c r="B169" s="186"/>
-      <c r="C169" s="186"/>
-      <c r="D169" s="186"/>
-      <c r="E169" s="186"/>
-      <c r="F169" s="186"/>
-      <c r="G169" s="186"/>
-      <c r="H169" s="186"/>
-      <c r="I169" s="186"/>
+      <c r="A169" s="184"/>
+      <c r="B169" s="184"/>
+      <c r="C169" s="184"/>
+      <c r="D169" s="184"/>
+      <c r="E169" s="184"/>
+      <c r="F169" s="184"/>
+      <c r="G169" s="184"/>
+      <c r="H169" s="184"/>
+      <c r="I169" s="184"/>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="55"/>
@@ -20940,7 +20594,7 @@
         <f>SUM(D172:D176)/(SUM(C172:C176))</f>
         <v>1.6666666666666667</v>
       </c>
-      <c r="I171" s="187">
+      <c r="I171" s="185">
         <f>GOT!G3</f>
         <v>39155</v>
       </c>
@@ -20963,7 +20617,7 @@
       <c r="E172" s="20"/>
       <c r="F172" s="20"/>
       <c r="G172" s="20"/>
-      <c r="I172" s="188"/>
+      <c r="I172" s="186"/>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="61" t="s">
@@ -20983,7 +20637,7 @@
       <c r="E173" s="20"/>
       <c r="F173" s="20"/>
       <c r="G173" s="20"/>
-      <c r="I173" s="188"/>
+      <c r="I173" s="186"/>
     </row>
     <row r="174" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="63" t="s">
@@ -21003,7 +20657,7 @@
       <c r="E174" s="20"/>
       <c r="F174" s="20"/>
       <c r="G174" s="20"/>
-      <c r="I174" s="188"/>
+      <c r="I174" s="186"/>
     </row>
     <row r="175" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="61" t="s">
@@ -21029,7 +20683,7 @@
         <v>2</v>
       </c>
       <c r="H175" s="20"/>
-      <c r="I175" s="188"/>
+      <c r="I175" s="186"/>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="66" t="s">
@@ -21053,16 +20707,36 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="A168:I169"/>
-    <mergeCell ref="I131:I135"/>
-    <mergeCell ref="I141:I145"/>
-    <mergeCell ref="I151:I155"/>
-    <mergeCell ref="I161:I165"/>
-    <mergeCell ref="A128:I129"/>
-    <mergeCell ref="A138:I139"/>
-    <mergeCell ref="A118:I119"/>
-    <mergeCell ref="A148:I149"/>
-    <mergeCell ref="A158:I159"/>
+    <mergeCell ref="I1:I5"/>
+    <mergeCell ref="A8:I9"/>
+    <mergeCell ref="A28:I29"/>
+    <mergeCell ref="I31:I35"/>
+    <mergeCell ref="A38:I39"/>
+    <mergeCell ref="I41:I45"/>
+    <mergeCell ref="T12:T16"/>
+    <mergeCell ref="T32:T36"/>
+    <mergeCell ref="L39:T40"/>
+    <mergeCell ref="T42:T46"/>
+    <mergeCell ref="I11:I15"/>
+    <mergeCell ref="A18:I19"/>
+    <mergeCell ref="I21:I25"/>
+    <mergeCell ref="T2:T6"/>
+    <mergeCell ref="L9:T10"/>
+    <mergeCell ref="L19:T20"/>
+    <mergeCell ref="T22:T26"/>
+    <mergeCell ref="L29:T30"/>
+    <mergeCell ref="BA2:BA3"/>
+    <mergeCell ref="BB2:BB3"/>
+    <mergeCell ref="AY4:AY7"/>
+    <mergeCell ref="BB4:BB7"/>
+    <mergeCell ref="AY8:AY11"/>
+    <mergeCell ref="BB8:BB11"/>
+    <mergeCell ref="BB12:BB15"/>
+    <mergeCell ref="AY16:AY19"/>
+    <mergeCell ref="BB16:BB19"/>
+    <mergeCell ref="AY20:AY23"/>
+    <mergeCell ref="BB20:BB23"/>
+    <mergeCell ref="AY12:AY15"/>
     <mergeCell ref="I171:I175"/>
     <mergeCell ref="A48:I49"/>
     <mergeCell ref="A58:I59"/>
@@ -21079,36 +20753,16 @@
     <mergeCell ref="I111:I115"/>
     <mergeCell ref="I121:I125"/>
     <mergeCell ref="A108:I109"/>
-    <mergeCell ref="BB12:BB15"/>
-    <mergeCell ref="AY16:AY19"/>
-    <mergeCell ref="BB16:BB19"/>
-    <mergeCell ref="AY20:AY23"/>
-    <mergeCell ref="BB20:BB23"/>
-    <mergeCell ref="AY12:AY15"/>
-    <mergeCell ref="BA2:BA3"/>
-    <mergeCell ref="BB2:BB3"/>
-    <mergeCell ref="AY4:AY7"/>
-    <mergeCell ref="BB4:BB7"/>
-    <mergeCell ref="AY8:AY11"/>
-    <mergeCell ref="BB8:BB11"/>
-    <mergeCell ref="T2:T6"/>
-    <mergeCell ref="L9:T10"/>
-    <mergeCell ref="L19:T20"/>
-    <mergeCell ref="T22:T26"/>
-    <mergeCell ref="L29:T30"/>
-    <mergeCell ref="I41:I45"/>
-    <mergeCell ref="T12:T16"/>
-    <mergeCell ref="T32:T36"/>
-    <mergeCell ref="L39:T40"/>
-    <mergeCell ref="T42:T46"/>
-    <mergeCell ref="I11:I15"/>
-    <mergeCell ref="A18:I19"/>
-    <mergeCell ref="I21:I25"/>
-    <mergeCell ref="I1:I5"/>
-    <mergeCell ref="A8:I9"/>
-    <mergeCell ref="A28:I29"/>
-    <mergeCell ref="I31:I35"/>
-    <mergeCell ref="A38:I39"/>
+    <mergeCell ref="A128:I129"/>
+    <mergeCell ref="A138:I139"/>
+    <mergeCell ref="A118:I119"/>
+    <mergeCell ref="A148:I149"/>
+    <mergeCell ref="A158:I159"/>
+    <mergeCell ref="A168:I169"/>
+    <mergeCell ref="I131:I135"/>
+    <mergeCell ref="I141:I145"/>
+    <mergeCell ref="I151:I155"/>
+    <mergeCell ref="I161:I165"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -21119,7 +20773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BG353"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="Y1" sqref="Y1:AG1"/>
     </sheetView>
   </sheetViews>
@@ -21153,31 +20807,31 @@
       <c r="B1" s="181"/>
       <c r="C1" s="181"/>
       <c r="Y1" s="120" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="Z1" s="120" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="AA1" s="120" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="AB1" s="120" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="AC1" s="120" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="AD1" s="120" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="AE1" s="120" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="AF1" s="120" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="AG1" s="120" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:59" x14ac:dyDescent="0.25">
@@ -38160,7 +37814,7 @@
       <c r="P9" s="137"/>
       <c r="Q9" s="137"/>
       <c r="R9" s="137" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="S9" s="180">
         <v>2002</v>
@@ -38218,7 +37872,7 @@
       <c r="P10" s="137"/>
       <c r="Q10" s="137"/>
       <c r="R10" s="165" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="S10" s="180"/>
       <c r="T10" s="180"/>
@@ -38227,7 +37881,7 @@
       <c r="P11" s="137"/>
       <c r="Q11" s="137"/>
       <c r="R11" s="162" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="S11" s="180"/>
       <c r="T11" s="180"/>
@@ -38269,7 +37923,7 @@
       <c r="P12" s="137"/>
       <c r="Q12" s="137"/>
       <c r="R12" s="162" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="S12" s="180"/>
       <c r="T12" s="180"/>
@@ -38314,7 +37968,7 @@
       <c r="P13" s="137"/>
       <c r="Q13" s="137"/>
       <c r="R13" s="165" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="S13" s="180">
         <v>2003</v>
@@ -38361,7 +38015,7 @@
       <c r="P14" s="137"/>
       <c r="Q14" s="137"/>
       <c r="R14" s="164" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="S14" s="180"/>
       <c r="T14" s="180"/>
@@ -38406,7 +38060,7 @@
       <c r="P15" s="137"/>
       <c r="Q15" s="137"/>
       <c r="R15" s="137" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="S15" s="180"/>
       <c r="T15" s="180"/>
@@ -38451,7 +38105,7 @@
       <c r="P16" s="137"/>
       <c r="Q16" s="137"/>
       <c r="R16" s="163" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="S16" s="180"/>
       <c r="T16" s="180"/>
@@ -38497,7 +38151,7 @@
       <c r="P17" s="137"/>
       <c r="Q17" s="137"/>
       <c r="R17" s="137" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="S17" s="180"/>
       <c r="T17" s="180"/>
@@ -38542,7 +38196,7 @@
       <c r="P18" s="137"/>
       <c r="Q18" s="137"/>
       <c r="R18" s="162" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="S18" s="180">
         <v>2004</v>
@@ -38589,7 +38243,7 @@
       <c r="P19" s="137"/>
       <c r="Q19" s="137"/>
       <c r="R19" s="137" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="S19" s="180"/>
       <c r="T19" s="180"/>
@@ -38635,7 +38289,7 @@
       <c r="P20" s="137"/>
       <c r="Q20" s="137"/>
       <c r="R20" s="171" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="S20" s="180"/>
       <c r="T20" s="180"/>
@@ -38681,7 +38335,7 @@
       <c r="P21" s="137"/>
       <c r="Q21" s="137"/>
       <c r="R21" s="170" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="S21" s="180"/>
       <c r="T21" s="180"/>
@@ -38727,7 +38381,7 @@
       <c r="P22" s="137"/>
       <c r="Q22" s="137"/>
       <c r="R22" s="137" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="S22" s="180"/>
       <c r="T22" s="180"/>
@@ -38772,7 +38426,7 @@
       <c r="P23" s="137"/>
       <c r="Q23" s="137"/>
       <c r="R23" s="164" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="S23" s="180">
         <v>2005</v>
@@ -38819,7 +38473,7 @@
       <c r="P24" s="137"/>
       <c r="Q24" s="137"/>
       <c r="R24" s="164" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="S24" s="180"/>
       <c r="T24" s="180"/>
@@ -38864,7 +38518,7 @@
       <c r="P25" s="137"/>
       <c r="Q25" s="137"/>
       <c r="R25" s="137" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="S25" s="180"/>
       <c r="T25" s="180"/>
@@ -38910,7 +38564,7 @@
       <c r="P26" s="137"/>
       <c r="Q26" s="137"/>
       <c r="R26" s="169" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="S26" s="180"/>
       <c r="T26" s="180"/>
@@ -38955,7 +38609,7 @@
       <c r="P27" s="137"/>
       <c r="Q27" s="137"/>
       <c r="R27" s="165" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="S27" s="180">
         <v>2006</v>
@@ -38966,7 +38620,7 @@
       <c r="P28" s="137"/>
       <c r="Q28" s="137"/>
       <c r="R28" s="162" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="S28" s="180"/>
       <c r="T28" s="180"/>
@@ -38975,7 +38629,7 @@
       <c r="P29" s="137"/>
       <c r="Q29" s="137"/>
       <c r="R29" s="137" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="S29" s="180"/>
       <c r="T29" s="180"/>
@@ -38984,7 +38638,7 @@
       <c r="P30" s="137"/>
       <c r="Q30" s="137"/>
       <c r="R30" s="162" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="S30" s="180">
         <v>2007</v>
@@ -38995,7 +38649,7 @@
       <c r="P31" s="137"/>
       <c r="Q31" s="137"/>
       <c r="R31" s="137" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="S31" s="180"/>
       <c r="T31" s="180"/>
@@ -39004,7 +38658,7 @@
       <c r="P32" s="137"/>
       <c r="Q32" s="137"/>
       <c r="R32" s="162" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="S32" s="180"/>
       <c r="T32" s="180"/>
@@ -39013,7 +38667,7 @@
       <c r="P33" s="137"/>
       <c r="Q33" s="137"/>
       <c r="R33" s="137" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="S33" s="180"/>
       <c r="T33" s="180"/>
@@ -39022,7 +38676,7 @@
       <c r="P34" s="137"/>
       <c r="Q34" s="137"/>
       <c r="R34" s="137" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="S34" s="180">
         <v>2008</v>
@@ -39033,7 +38687,7 @@
       <c r="P35" s="137"/>
       <c r="Q35" s="137"/>
       <c r="R35" s="164" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="S35" s="180"/>
       <c r="T35" s="180"/>
@@ -39042,7 +38696,7 @@
       <c r="P36" s="137"/>
       <c r="Q36" s="137"/>
       <c r="R36" s="164" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="S36" s="180"/>
       <c r="T36" s="180"/>
@@ -39051,7 +38705,7 @@
       <c r="P37" s="137"/>
       <c r="Q37" s="137"/>
       <c r="R37" s="137" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="S37" s="180">
         <v>2009</v>
@@ -39062,7 +38716,7 @@
       <c r="P38" s="137"/>
       <c r="Q38" s="137"/>
       <c r="R38" s="137" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="S38" s="180"/>
       <c r="T38" s="180"/>
@@ -39072,7 +38726,7 @@
       <c r="P39" s="137"/>
       <c r="Q39" s="137"/>
       <c r="R39" s="137" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="S39" s="180"/>
       <c r="T39" s="180"/>
@@ -39082,7 +38736,7 @@
       <c r="P40" s="137"/>
       <c r="Q40" s="137"/>
       <c r="R40" s="137" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="S40" s="180">
         <v>2012</v>
@@ -39093,7 +38747,7 @@
       <c r="P41" s="137"/>
       <c r="Q41" s="137"/>
       <c r="R41" s="137" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="S41" s="180">
         <v>2014</v>
@@ -39104,7 +38758,7 @@
       <c r="P42" s="137"/>
       <c r="Q42" s="137"/>
       <c r="R42" s="137" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="S42" s="180">
         <v>2015</v>
@@ -39115,7 +38769,7 @@
       <c r="P43" s="137"/>
       <c r="Q43" s="137"/>
       <c r="R43" s="137" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="S43" s="180">
         <v>2017</v>
@@ -39124,11 +38778,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="S9:T12"/>
-    <mergeCell ref="S13:T17"/>
-    <mergeCell ref="S18:T22"/>
-    <mergeCell ref="S23:T26"/>
     <mergeCell ref="S41:T41"/>
     <mergeCell ref="S42:T42"/>
     <mergeCell ref="S43:T43"/>
@@ -39137,6 +38786,11 @@
     <mergeCell ref="S34:T36"/>
     <mergeCell ref="S37:T39"/>
     <mergeCell ref="S40:T40"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="S9:T12"/>
+    <mergeCell ref="S13:T17"/>
+    <mergeCell ref="S18:T22"/>
+    <mergeCell ref="S23:T26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -39272,7 +38926,7 @@
       <c r="G11" s="137"/>
       <c r="H11" s="137"/>
       <c r="I11" s="137" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="J11" s="137"/>
       <c r="K11" s="137"/>
@@ -39301,7 +38955,7 @@
       <c r="G12" s="137"/>
       <c r="H12" s="137"/>
       <c r="I12" s="137" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="J12" s="137"/>
       <c r="K12" s="137"/>
@@ -39328,7 +38982,7 @@
       <c r="G13" s="137"/>
       <c r="H13" s="137"/>
       <c r="I13" s="137" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="J13" s="137"/>
       <c r="K13" s="137"/>
@@ -39355,7 +39009,7 @@
       <c r="G14" s="137"/>
       <c r="H14" s="137"/>
       <c r="I14" s="137" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="J14" s="137"/>
       <c r="K14" s="137"/>
@@ -39382,7 +39036,7 @@
       <c r="G15" s="137"/>
       <c r="H15" s="137"/>
       <c r="I15" s="137" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="J15" s="137"/>
       <c r="K15" s="137"/>
@@ -39411,7 +39065,7 @@
       <c r="G16" s="137"/>
       <c r="H16" s="137"/>
       <c r="I16" s="137" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="J16" s="137"/>
       <c r="K16" s="137"/>
@@ -39438,7 +39092,7 @@
       <c r="G17" s="137"/>
       <c r="H17" s="137"/>
       <c r="I17" s="137" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="J17" s="137"/>
       <c r="K17" s="137"/>
@@ -39465,7 +39119,7 @@
       <c r="G18" s="137"/>
       <c r="H18" s="137"/>
       <c r="I18" s="137" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="J18" s="137"/>
       <c r="K18" s="137"/>
@@ -39492,7 +39146,7 @@
       <c r="G19" s="137"/>
       <c r="H19" s="137"/>
       <c r="I19" s="137" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="J19" s="137"/>
       <c r="K19" s="137"/>
@@ -39519,7 +39173,7 @@
       <c r="G20" s="137"/>
       <c r="H20" s="137"/>
       <c r="I20" s="137" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="J20" s="137"/>
       <c r="K20" s="137"/>
@@ -39548,7 +39202,7 @@
       <c r="G21" s="137"/>
       <c r="H21" s="137"/>
       <c r="I21" s="137" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="J21" s="137"/>
       <c r="K21" s="137"/>
@@ -39575,7 +39229,7 @@
       <c r="G22" s="137"/>
       <c r="H22" s="137"/>
       <c r="I22" s="137" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="J22" s="137"/>
       <c r="K22" s="137"/>
@@ -39602,7 +39256,7 @@
       <c r="G23" s="137"/>
       <c r="H23" s="137"/>
       <c r="I23" s="137" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="J23" s="137"/>
       <c r="K23" s="137"/>
@@ -39629,7 +39283,7 @@
       <c r="G24" s="137"/>
       <c r="H24" s="137"/>
       <c r="I24" s="137" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="J24" s="137"/>
       <c r="K24" s="137"/>
@@ -39656,7 +39310,7 @@
       <c r="G25" s="137"/>
       <c r="H25" s="137"/>
       <c r="I25" s="137" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="J25" s="137"/>
       <c r="K25" s="137"/>
@@ -39685,7 +39339,7 @@
       <c r="G26" s="137"/>
       <c r="H26" s="137"/>
       <c r="I26" s="137" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="J26" s="137"/>
       <c r="K26" s="137"/>
@@ -39712,7 +39366,7 @@
       <c r="G27" s="137"/>
       <c r="H27" s="137"/>
       <c r="I27" s="137" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="J27" s="137"/>
       <c r="K27" s="137"/>
@@ -39729,7 +39383,7 @@
       <c r="G28" s="137"/>
       <c r="H28" s="137"/>
       <c r="I28" s="137" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="J28" s="137"/>
       <c r="K28" s="137"/>
@@ -39746,7 +39400,7 @@
       <c r="G29" s="137"/>
       <c r="H29" s="137"/>
       <c r="I29" s="137" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="J29" s="137"/>
       <c r="K29" s="137"/>
@@ -39765,7 +39419,7 @@
       <c r="G30" s="137"/>
       <c r="H30" s="137"/>
       <c r="I30" s="137" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="J30" s="137"/>
       <c r="K30" s="137"/>
@@ -39782,7 +39436,7 @@
       <c r="G31" s="137"/>
       <c r="H31" s="137"/>
       <c r="I31" s="137" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="J31" s="137"/>
       <c r="K31" s="137"/>
@@ -39799,7 +39453,7 @@
       <c r="G32" s="137"/>
       <c r="H32" s="137"/>
       <c r="I32" s="137" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="J32" s="137"/>
       <c r="K32" s="137"/>
@@ -39818,7 +39472,7 @@
       <c r="G33" s="137"/>
       <c r="H33" s="137"/>
       <c r="I33" s="137" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="J33" s="137"/>
       <c r="K33" s="137"/>
@@ -39835,7 +39489,7 @@
       <c r="G34" s="137"/>
       <c r="H34" s="137"/>
       <c r="I34" s="137" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="J34" s="137"/>
       <c r="K34" s="137"/>
@@ -39852,7 +39506,7 @@
       <c r="G35" s="137"/>
       <c r="H35" s="137"/>
       <c r="I35" s="137" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="J35" s="137"/>
       <c r="K35" s="137"/>
@@ -39869,7 +39523,7 @@
       <c r="G36" s="137"/>
       <c r="H36" s="137"/>
       <c r="I36" s="137" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="J36" s="137"/>
       <c r="K36" s="137"/>
@@ -39888,7 +39542,7 @@
       <c r="G37" s="137"/>
       <c r="H37" s="137"/>
       <c r="I37" s="137" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="J37" s="137"/>
       <c r="K37" s="137"/>
@@ -39905,7 +39559,7 @@
       <c r="G38" s="137"/>
       <c r="H38" s="137"/>
       <c r="I38" s="137" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
       <c r="J38" s="137"/>
       <c r="K38" s="137"/>
@@ -39922,7 +39576,7 @@
       <c r="G39" s="137"/>
       <c r="H39" s="137"/>
       <c r="I39" s="137" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="J39" s="137"/>
       <c r="K39" s="137"/>
@@ -39941,7 +39595,7 @@
       <c r="G40" s="137"/>
       <c r="H40" s="137"/>
       <c r="I40" s="137" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="J40" s="137"/>
       <c r="K40" s="137"/>
@@ -39958,7 +39612,7 @@
       <c r="G41" s="137"/>
       <c r="H41" s="137"/>
       <c r="I41" s="137" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="J41" s="137"/>
       <c r="K41" s="137"/>
@@ -39975,7 +39629,7 @@
       <c r="G42" s="137"/>
       <c r="H42" s="137"/>
       <c r="I42" s="137" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="J42" s="137"/>
       <c r="K42" s="137"/>
@@ -39994,7 +39648,7 @@
       <c r="G43" s="137"/>
       <c r="H43" s="137"/>
       <c r="I43" s="137" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="J43" s="137"/>
       <c r="K43" s="137"/>
@@ -40013,7 +39667,7 @@
       <c r="G44" s="137"/>
       <c r="H44" s="137"/>
       <c r="I44" s="137" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="J44" s="137"/>
       <c r="K44" s="137"/>
@@ -40032,7 +39686,7 @@
       <c r="G45" s="137"/>
       <c r="H45" s="137"/>
       <c r="I45" s="137" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="J45" s="137"/>
       <c r="K45" s="137"/>
@@ -40067,6 +39721,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101007D2ED3CE96C13443B502633C8A95469B" ma:contentTypeVersion="0" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="f85a63a8cdffcff2cdbd17d1e9b5509e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="65db0ef88017f3ca28aa19d4b0cf03fd">
     <xsd:element name="properties">
@@ -40180,32 +39849,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1186F27-5F44-40C2-B09E-CA97BC280255}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B052E13-3436-4068-9DA3-8DA91858E98B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
@@ -40220,9 +39867,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4B052E13-3436-4068-9DA3-8DA91858E98B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1186F27-5F44-40C2-B09E-CA97BC280255}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>